<commit_message>
Added article A dynamic metric to measure the time required to execute mentally a program
</commit_message>
<xml_diff>
--- a/dataset-cpx.xlsx
+++ b/dataset-cpx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/these/studies/cpx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1069429-2E78-C344-97BC-11D7FFFEFC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A5CBF6-416E-F543-9D1E-75E5B083B173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{E3999CCB-9ED0-3445-84E9-42CD1661CA3C}"/>
+    <workbookView xWindow="35840" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{E3999CCB-9ED0-3445-84E9-42CD1661CA3C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -61,6 +61,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Feuil37!$B$7:$C$42</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">siegmund2012!$C$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">siegmund2012!$C$4:$C$22</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">siegmund2012!$G$3</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">siegmund2012!$G$4:$G$22</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">siegmund2012!$C$3</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">siegmund2012!$C$4:$C$22</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">siegmund2012!$G$3</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">siegmund2012!$G$4:$G$22</definedName>
     <definedName name="xdata1" hidden="1">#REF!</definedName>
     <definedName name="xdata2" hidden="1">#REF!</definedName>
     <definedName name="xdata3" hidden="1">#REF!</definedName>
@@ -149,8 +157,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="509">
   <si>
     <t>snippet_id</t>
   </si>
@@ -6187,6 +6217,9 @@
   </si>
   <si>
     <t>dyn2</t>
+  </si>
+  <si>
+    <t>Linear regression line</t>
   </si>
 </sst>
 </file>
@@ -6363,7 +6396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6421,6 +6454,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6555,7 +6594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6775,6 +6814,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7508,6 +7553,1014 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>dyn2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>siegmund2012!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dyn2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>siegmund2012!$G$4:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4.8948</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7837939390651911</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3121798400000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.704923999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7900520000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6073685280000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8864000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.1806567180919743</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.0659999999999989</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.976</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8332000000000006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4130162525952006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.1000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.6915907722453642</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.4580000000000011</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.1128912</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.7813413250560011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>siegmund2012!$C$4:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>68.014414634146334</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.26741463414632</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>154.64156097560979</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>211.48453658536584</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.510951219512179</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66.048609756097534</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104.82602439024393</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65.420853658536572</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42.585804878048783</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65.473780487804873</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59.81002439024391</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37.425292682926823</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>48.394707317073163</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20.50239024390244</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.988414634146352</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>145.23982926829271</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.621829268292686</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89.939219512195123</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>54.500707317073157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-92CD-5241-A85C-4FD114D62F15}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1828947583"/>
+        <c:axId val="1518830015"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1828947583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1518830015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1518830015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1828947583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>peitek2021!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dyn 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-847A-994B-A457-CD471C709299}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-847A-994B-A457-CD471C709299}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="12700">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000014-847A-994B-A457-CD471C709299}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-847A-994B-A457-CD471C709299}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-847A-994B-A457-CD471C709299}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000018-847A-994B-A457-CD471C709299}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>peitek2021!$C$4:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>41.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.869999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.65</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36.979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>31.74</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28.54</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>34.83</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>peitek2021!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>11.744000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.183487999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.699563093333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.360000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.160000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.2889600000000012</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.3591999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.9640000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.4496000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.4600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.368000000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-847A-994B-A457-CD471C709299}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="572206560"/>
+        <c:axId val="572188096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="572206560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572188096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="572188096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572206560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:overlay val="0"/>
@@ -7913,7 +8966,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -8331,7 +9384,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -8985,7 +10038,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{217A56BC-66ED-8E46-A962-686851683D40}" type="CELLRANGE">
+                    <a:fld id="{2F39DA6A-E70F-004D-A8E4-455A9706DC17}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9018,7 +10071,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29F726E1-919A-CC40-A8CE-839BC5B9E7DB}" type="CELLRANGE">
+                    <a:fld id="{51348929-3CE8-904D-8782-246BF01051EB}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9051,7 +10104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F4BDB46-738C-864A-8D31-7983B663811E}" type="CELLRANGE">
+                    <a:fld id="{812BA8D4-10F9-2246-8E72-BC438B869F21}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9084,7 +10137,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19B902FD-A5C0-0340-B7A5-386CC680DB09}" type="CELLRANGE">
+                    <a:fld id="{F0F3FBDB-20E5-CE41-9CD9-9F6DA2B6A509}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9117,7 +10170,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51F2BA61-F0AD-E846-9023-351540B12AA9}" type="CELLRANGE">
+                    <a:fld id="{9FBD59BC-295E-6A45-A49E-7BFDB16F6541}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9150,7 +10203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF8EE59F-DF8B-814F-AB88-C272EADF37B9}" type="CELLRANGE">
+                    <a:fld id="{C7E10F74-FF33-5F4E-A291-CBF4B32EFF9B}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9183,7 +10236,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D881C090-EF1E-3243-BC3E-1D190F82F211}" type="CELLRANGE">
+                    <a:fld id="{3DE4E1CA-077C-C740-A9D1-D4630E9A6A2B}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9216,7 +10269,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD2D226D-7BF0-BF4F-AFCF-38DE8E5A6BFD}" type="CELLRANGE">
+                    <a:fld id="{3E324EC8-9509-9142-A4DF-178DE429EA5A}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9249,7 +10302,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{272DEF72-8819-2042-9526-DD0904C1FE84}" type="CELLRANGE">
+                    <a:fld id="{3A1387D7-EFB1-054E-AACF-929E55FC7FBD}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9282,7 +10335,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11E39833-98EA-6F41-A150-0A38C61ECA75}" type="CELLRANGE">
+                    <a:fld id="{847C2912-4AE9-2B4A-8612-651823491E89}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9315,7 +10368,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E36AA6C-BD00-F14A-B325-6767E2835DC8}" type="CELLRANGE">
+                    <a:fld id="{A1824833-361C-0043-950A-3A2A1D29199D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9348,7 +10401,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77BC205A-7F17-3B40-926B-7375F6B8D13D}" type="CELLRANGE">
+                    <a:fld id="{E6A36DEE-156F-3C46-8796-44474D28D323}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9381,7 +10434,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{96865374-F17C-0F48-B4EB-988F91AF19B4}" type="CELLRANGE">
+                    <a:fld id="{6279345F-23FB-EC4F-AB0B-E32FA94A3D88}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9414,7 +10467,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51B6B16A-3980-764F-A805-08C618A6A68F}" type="CELLRANGE">
+                    <a:fld id="{3084130C-DCF6-F246-B0CC-B0BE97F0A1C5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9447,7 +10500,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D47D70F-D2CE-9F4B-ABEF-3CEE95BB2C63}" type="CELLRANGE">
+                    <a:fld id="{F1842C9B-B8B9-3747-A93C-1FD3834DDB66}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9480,7 +10533,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CE404CA-C2CF-A44B-BA5B-0B2866BFF3EA}" type="CELLRANGE">
+                    <a:fld id="{4DD2E44E-D086-E042-9596-A11826EB5F63}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9513,7 +10566,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E00FFDCD-2067-8647-8D41-8B9BF9E22CA9}" type="CELLRANGE">
+                    <a:fld id="{99165BB0-3594-4840-828C-49DA02FD464F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9546,7 +10599,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C458C524-0560-E34E-BA43-171667EA6075}" type="CELLRANGE">
+                    <a:fld id="{C697E4E9-7030-E847-9A41-B68DA8656610}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9579,7 +10632,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4814A77-C47D-664D-B168-B8898DCD4180}" type="CELLRANGE">
+                    <a:fld id="{44DCBF68-1548-F04E-B0E7-EB1A600AFDC0}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9612,7 +10665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBF22F93-FD5E-104B-B3DA-E128B61A0B3B}" type="CELLRANGE">
+                    <a:fld id="{4A0650A8-834E-2543-AA9A-8673BB3F5FC1}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9645,7 +10698,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A303A353-FCC0-944C-A58A-A0DB8F39775B}" type="CELLRANGE">
+                    <a:fld id="{93F49A16-9BFA-6547-B498-DA637D6C51CB}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9678,7 +10731,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F400C187-677C-944B-8ABB-8DFF20743D62}" type="CELLRANGE">
+                    <a:fld id="{E9385C19-D00E-5C46-A844-228595570F8C}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -9711,7 +10764,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DD04408-4654-A741-A2CD-F54FA8B8307B}" type="CELLRANGE">
+                    <a:fld id="{54E06FA0-E2D3-5C4D-AEBD-0F6C3D52159E}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -12892,8 +13945,34 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>sonarqube</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12934,17 +14013,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>peitek2021!$F$3</c:f>
+              <c:f>siegmund2012!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>dyn 1</c:v>
+                  <c:v>sonarqube</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -12965,150 +14044,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000019-847A-994B-A457-CD471C709299}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000015-847A-994B-A457-CD471C709299}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="12700">
-                  <a:solidFill>
-                    <a:srgbClr val="FF0000"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000014-847A-994B-A457-CD471C709299}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="11"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000016-847A-994B-A457-CD471C709299}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="12"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000017-847A-994B-A457-CD471C709299}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="13"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="8"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000018-847A-994B-A457-CD471C709299}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -13123,131 +14058,134 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:forward val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>peitek2021!$C$4:$C$19</c:f>
+              <c:f>siegmund2012!$D$4:$D$22</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>41.24</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.33</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.95</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.869999999999997</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.82</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.78</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.52</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.869999999999997</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.65</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.979999999999997</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24.25</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31.74</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.54</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.83</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.05</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>peitek2021!$F$4:$F$19</c:f>
+              <c:f>siegmund2012!$C$4:$C$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>11.744000000000002</c:v>
+                  <c:v>68.014414634146334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.183487999999997</c:v>
+                  <c:v>100.26741463414632</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.699563093333332</c:v>
+                  <c:v>154.64156097560979</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19</c:v>
+                  <c:v>211.48453658536584</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.360000000000001</c:v>
+                  <c:v>70.510951219512179</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.160000000000004</c:v>
+                  <c:v>66.048609756097534</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>104.82602439024393</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.8000000000000007</c:v>
+                  <c:v>65.420853658536572</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.2889600000000012</c:v>
+                  <c:v>42.585804878048783</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.36</c:v>
+                  <c:v>65.473780487804873</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.3591999999999995</c:v>
+                  <c:v>59.81002439024391</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9640000000000004</c:v>
+                  <c:v>37.425292682926823</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4496000000000002</c:v>
+                  <c:v>48.394707317073163</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4600000000000009</c:v>
+                  <c:v>20.50239024390244</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.368000000000004</c:v>
+                  <c:v>99.988414634146352</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>145.23982926829271</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80.621829268292686</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89.939219512195123</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>54.500707317073157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13255,7 +14193,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-847A-994B-A457-CD471C709299}"/>
+              <c16:uniqueId val="{00000000-92CD-5241-A85C-4FD114D62F15}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13267,17 +14205,79 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="572206560"/>
-        <c:axId val="572188096"/>
+        <c:axId val="1828947583"/>
+        <c:axId val="1518830015"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="572206560"/>
+        <c:axId val="1828947583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="20"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1518830015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1518830015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -13329,69 +14329,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572188096"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="572188096"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="572206560"/>
+        <c:crossAx val="1828947583"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13406,6 +14344,7 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -13561,6 +14500,86 @@
 </file>
 
 <file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -15456,6 +16475,1038 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -20399,6 +22450,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>89370</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>492242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>545630</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>4127499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2F70887-67EA-EE4E-8696-6E6B17E51B45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>492242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>204612</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>4139259</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A12568C6-CA78-7846-B537-178B755DA014}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -20852,6 +22975,578 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/themeOverride1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
+<file path=xl/theme/themeOverride2.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A7" dT="2021-07-11T11:22:41.13" personId="{A4C9A5BD-8491-454E-A1E9-D85386424885}" id="{6AC9C0CF-436C-2D4D-8C21-20009B6E65B2}">
@@ -33042,10 +35737,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B752191-782E-EA48-B322-664FAB9CF9B3}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="B1:H53"/>
+  <dimension ref="B1:AH53"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -33058,10 +35753,12 @@
     <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="18" width="10.83203125" style="1"/>
+    <col min="19" max="19" width="4.1640625" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="19">
+    <row r="1" spans="2:34" ht="19">
       <c r="B1" s="106" t="s">
         <v>474</v>
       </c>
@@ -33071,7 +35768,14 @@
       <c r="F1" s="106"/>
       <c r="G1" s="106"/>
     </row>
-    <row r="3" spans="2:8">
+    <row r="2" spans="2:34">
+      <c r="T2" s="121" t="s">
+        <v>508</v>
+      </c>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+    </row>
+    <row r="3" spans="2:34">
       <c r="B3" s="72" t="s">
         <v>502</v>
       </c>
@@ -33093,8 +35797,55 @@
         <v>dyn2</v>
       </c>
       <c r="H3" s="99"/>
-    </row>
-    <row r="4" spans="2:8">
+      <c r="T3" s="1" t="str">
+        <f>D3</f>
+        <v>sonarqube</v>
+      </c>
+      <c r="U3" s="1" cm="1">
+        <f t="array" ref="U3:V3">LINEST(D4:D22,C4:C22)</f>
+        <v>2.4558162269338261E-2</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0.68727428091925669</v>
+      </c>
+      <c r="X3" s="14" t="str">
+        <f>D3</f>
+        <v>sonarqube</v>
+      </c>
+      <c r="Y3" s="14" t="str">
+        <f>E3</f>
+        <v>genese_cpx</v>
+      </c>
+      <c r="Z3" s="14" t="str">
+        <f>F3</f>
+        <v>dyn1</v>
+      </c>
+      <c r="AA3" s="14" t="str">
+        <f>G3</f>
+        <v>dyn2</v>
+      </c>
+      <c r="AC3" s="14" t="str">
+        <f>D3</f>
+        <v>sonarqube</v>
+      </c>
+      <c r="AD3" s="14" t="str">
+        <f>E3</f>
+        <v>genese_cpx</v>
+      </c>
+      <c r="AE3" s="14" t="str">
+        <f>F3</f>
+        <v>dyn1</v>
+      </c>
+      <c r="AF3" s="14" t="str">
+        <f>G3</f>
+        <v>dyn2</v>
+      </c>
+      <c r="AH3" s="1">
+        <f>STDEV(X4:X22)</f>
+        <v>25.675427112967437</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34">
       <c r="B4" s="37">
         <v>1</v>
       </c>
@@ -33116,8 +35867,51 @@
         <v>4.8948</v>
       </c>
       <c r="H4" s="99"/>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="T4" s="1" t="str">
+        <f>E3</f>
+        <v>genese_cpx</v>
+      </c>
+      <c r="U4" s="1" cm="1">
+        <f t="array" ref="U4:V4">LINEST(E4:E22,C4:C22)</f>
+        <v>5.5463678990432835E-2</v>
+      </c>
+      <c r="V4" s="1">
+        <v>6.7027076730524611</v>
+      </c>
+      <c r="X4" s="1">
+        <f>$D4*$U$10+$V$10</f>
+        <v>61.416918832752614</v>
+      </c>
+      <c r="Y4" s="1">
+        <f>E4*$U$11+$V$11</f>
+        <v>58.202273239029132</v>
+      </c>
+      <c r="Z4" s="1">
+        <f>F4*$U$12+$V$12</f>
+        <v>51.752996067965306</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>G4*$U$13+$V$13</f>
+        <v>58.230202971233552</v>
+      </c>
+      <c r="AC4" s="1">
+        <f>ABS($C4-X4)</f>
+        <v>6.5974958013937197</v>
+      </c>
+      <c r="AD4" s="1">
+        <f t="shared" ref="AD4:AF19" si="0">ABS($C4-Y4)</f>
+        <v>9.8121413951172016</v>
+      </c>
+      <c r="AE4" s="1">
+        <f t="shared" si="0"/>
+        <v>16.261418566181028</v>
+      </c>
+      <c r="AF4" s="1">
+        <f t="shared" si="0"/>
+        <v>9.7842116629127815</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34">
       <c r="B5" s="37">
         <v>2</v>
       </c>
@@ -33139,8 +35933,51 @@
         <v>7.7837939390651911</v>
       </c>
       <c r="H5" s="99"/>
-    </row>
-    <row r="6" spans="2:8">
+      <c r="T5" s="1" t="str">
+        <f>F3</f>
+        <v>dyn1</v>
+      </c>
+      <c r="U5" s="1" cm="1">
+        <f t="array" ref="U5:V5">LINEST(F4:F22,C4:C22)</f>
+        <v>7.6128649226312323E-2</v>
+      </c>
+      <c r="V5" s="1">
+        <v>1.4159069751836109</v>
+      </c>
+      <c r="X5" s="1">
+        <f>$D5*$U$10+$V$10</f>
+        <v>112.1775137456446</v>
+      </c>
+      <c r="Y5" s="1">
+        <f>E5*$U$11+$V$11</f>
+        <v>121.17951911274326</v>
+      </c>
+      <c r="Z5" s="1">
+        <f>F5*$U$12+$V$12</f>
+        <v>113.07798598541521</v>
+      </c>
+      <c r="AA5" s="1">
+        <f>G5*$U$13+$V$13</f>
+        <v>114.54182119618963</v>
+      </c>
+      <c r="AC5" s="1">
+        <f t="shared" ref="AC5:AC22" si="1">ABS($C5-X5)</f>
+        <v>11.910099111498283</v>
+      </c>
+      <c r="AD5" s="1">
+        <f t="shared" si="0"/>
+        <v>20.912104478596945</v>
+      </c>
+      <c r="AE5" s="1">
+        <f t="shared" si="0"/>
+        <v>12.810571351268891</v>
+      </c>
+      <c r="AF5" s="1">
+        <f t="shared" si="0"/>
+        <v>14.27440656204331</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34">
       <c r="B6" s="37">
         <v>4</v>
       </c>
@@ -33162,8 +35999,51 @@
         <v>9.3121798400000007</v>
       </c>
       <c r="H6" s="99"/>
-    </row>
-    <row r="7" spans="2:8">
+      <c r="T6" s="1" t="str">
+        <f>G3</f>
+        <v>dyn2</v>
+      </c>
+      <c r="U6" s="1" cm="1">
+        <f t="array" ref="U6:V6">LINEST(G4:G22,C4:C22)</f>
+        <v>4.4544978836098509E-2</v>
+      </c>
+      <c r="V6" s="1">
+        <v>2.4714422904012738</v>
+      </c>
+      <c r="X6" s="1">
+        <f>$D6*$U$10+$V$10</f>
+        <v>137.55781120209062</v>
+      </c>
+      <c r="Y6" s="1">
+        <f>E6*$U$11+$V$11</f>
+        <v>106.13185859424519</v>
+      </c>
+      <c r="Z6" s="1">
+        <f>F6*$U$12+$V$12</f>
+        <v>162.09344766569455</v>
+      </c>
+      <c r="AA6" s="1">
+        <f>G6*$U$13+$V$13</f>
+        <v>144.33277443775143</v>
+      </c>
+      <c r="AC6" s="1">
+        <f t="shared" si="1"/>
+        <v>17.083749773519173</v>
+      </c>
+      <c r="AD6" s="1">
+        <f t="shared" si="0"/>
+        <v>48.509702381364605</v>
+      </c>
+      <c r="AE6" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4518866900847627</v>
+      </c>
+      <c r="AF6" s="1">
+        <f t="shared" si="0"/>
+        <v>10.308786537858367</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34">
       <c r="B7" s="37">
         <v>5</v>
       </c>
@@ -33185,8 +36065,40 @@
         <v>11.704923999999998</v>
       </c>
       <c r="H7" s="99"/>
-    </row>
-    <row r="8" spans="2:8">
+      <c r="X7" s="1">
+        <f>$D7*$U$10+$V$10</f>
+        <v>112.1775137456446</v>
+      </c>
+      <c r="Y7" s="1">
+        <f>E7*$U$11+$V$11</f>
+        <v>100.00133023485711</v>
+      </c>
+      <c r="Z7" s="1">
+        <f>F7*$U$12+$V$12</f>
+        <v>189.67856056512687</v>
+      </c>
+      <c r="AA7" s="1">
+        <f>G7*$U$13+$V$13</f>
+        <v>190.97160390220904</v>
+      </c>
+      <c r="AC7" s="1">
+        <f t="shared" si="1"/>
+        <v>99.307022839721242</v>
+      </c>
+      <c r="AD7" s="1">
+        <f t="shared" si="0"/>
+        <v>111.48320635050874</v>
+      </c>
+      <c r="AE7" s="1">
+        <f t="shared" si="0"/>
+        <v>21.805976020238973</v>
+      </c>
+      <c r="AF7" s="1">
+        <f t="shared" si="0"/>
+        <v>20.512932683156805</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34">
       <c r="B8" s="37">
         <v>6</v>
       </c>
@@ -33208,8 +36120,40 @@
         <v>4.7900520000000002</v>
       </c>
       <c r="H8" s="99"/>
-    </row>
-    <row r="9" spans="2:8">
+      <c r="X8" s="1">
+        <f>$D8*$U$10+$V$10</f>
+        <v>61.416918832752614</v>
+      </c>
+      <c r="Y8" s="1">
+        <f>E8*$U$11+$V$11</f>
+        <v>59.87423551886225</v>
+      </c>
+      <c r="Z8" s="1">
+        <f>F8*$U$12+$V$12</f>
+        <v>53.723361275067617</v>
+      </c>
+      <c r="AA8" s="1">
+        <f>G8*$U$13+$V$13</f>
+        <v>56.18847858196871</v>
+      </c>
+      <c r="AC8" s="1">
+        <f t="shared" si="1"/>
+        <v>9.0940323867595652</v>
+      </c>
+      <c r="AD8" s="1">
+        <f t="shared" si="0"/>
+        <v>10.63671570064993</v>
+      </c>
+      <c r="AE8" s="1">
+        <f t="shared" si="0"/>
+        <v>16.787589944444562</v>
+      </c>
+      <c r="AF8" s="1">
+        <f t="shared" si="0"/>
+        <v>14.32247263754347</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34">
       <c r="B9" s="37">
         <v>7</v>
       </c>
@@ -33231,8 +36175,45 @@
         <v>6.6073685280000003</v>
       </c>
       <c r="H9" s="99"/>
-    </row>
-    <row r="10" spans="2:8">
+      <c r="T9" s="121" t="s">
+        <v>508</v>
+      </c>
+      <c r="U9" s="121"/>
+      <c r="V9" s="121"/>
+      <c r="X9" s="1">
+        <f>$D9*$U$10+$V$10</f>
+        <v>86.797216289198616</v>
+      </c>
+      <c r="Y9" s="1">
+        <f>E9*$U$11+$V$11</f>
+        <v>73.249933757527202</v>
+      </c>
+      <c r="Z9" s="1">
+        <f>F9*$U$12+$V$12</f>
+        <v>98.54916973664514</v>
+      </c>
+      <c r="AA9" s="1">
+        <f>G9*$U$13+$V$13</f>
+        <v>91.611202435710055</v>
+      </c>
+      <c r="AC9" s="1">
+        <f t="shared" si="1"/>
+        <v>20.748606533101082</v>
+      </c>
+      <c r="AD9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2013240014296684</v>
+      </c>
+      <c r="AE9" s="1">
+        <f t="shared" si="0"/>
+        <v>32.500559980547607</v>
+      </c>
+      <c r="AF9" s="1">
+        <f t="shared" si="0"/>
+        <v>25.562592679612521</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34">
       <c r="B10" s="103">
         <v>8</v>
       </c>
@@ -33254,8 +36235,51 @@
         <v>6.8864000000000001</v>
       </c>
       <c r="H10" s="99"/>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="T10" s="1" t="str">
+        <f>T3</f>
+        <v>sonarqube</v>
+      </c>
+      <c r="U10" s="1" cm="1">
+        <f t="array" ref="U10:V10">LINEST(C4:C22,D4:D22)</f>
+        <v>12.690148728222999</v>
+      </c>
+      <c r="V10" s="1">
+        <v>48.726770104529614</v>
+      </c>
+      <c r="X10" s="1">
+        <f>$D10*$U$10+$V$10</f>
+        <v>61.416918832752614</v>
+      </c>
+      <c r="Y10" s="1">
+        <f>E10*$U$11+$V$11</f>
+        <v>61.546197798695374</v>
+      </c>
+      <c r="Z10" s="1">
+        <f>F10*$U$12+$V$12</f>
+        <v>90.175117606460319</v>
+      </c>
+      <c r="AA10" s="1">
+        <f>G10*$U$13+$V$13</f>
+        <v>97.050020950191168</v>
+      </c>
+      <c r="AC10" s="1">
+        <f t="shared" si="1"/>
+        <v>43.409105557491316</v>
+      </c>
+      <c r="AD10" s="1">
+        <f t="shared" si="0"/>
+        <v>43.279826591548556</v>
+      </c>
+      <c r="AE10" s="1">
+        <f t="shared" si="0"/>
+        <v>14.650906783783611</v>
+      </c>
+      <c r="AF10" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7760034400527616</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34">
       <c r="B11" s="103">
         <v>9</v>
       </c>
@@ -33277,8 +36301,51 @@
         <v>5.1806567180919743</v>
       </c>
       <c r="H11" s="99"/>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="T11" s="1" t="str">
+        <f t="shared" ref="T11:T13" si="2">T4</f>
+        <v>genese_cpx</v>
+      </c>
+      <c r="U11" s="1" cm="1">
+        <f t="array" ref="U11:V11">LINEST(C4:C22,E4:E22)</f>
+        <v>5.5732075994437276</v>
+      </c>
+      <c r="V11" s="1">
+        <v>20.304461562811788</v>
+      </c>
+      <c r="X11" s="1">
+        <f>$D11*$U$10+$V$10</f>
+        <v>86.797216289198616</v>
+      </c>
+      <c r="Y11" s="1">
+        <f>E11*$U$11+$V$11</f>
+        <v>69.906009197860968</v>
+      </c>
+      <c r="Z11" s="1">
+        <f>F11*$U$12+$V$12</f>
+        <v>78.96262041061054</v>
+      </c>
+      <c r="AA11" s="1">
+        <f>G11*$U$13+$V$13</f>
+        <v>63.802057643051512</v>
+      </c>
+      <c r="AC11" s="1">
+        <f t="shared" si="1"/>
+        <v>21.376362630662044</v>
+      </c>
+      <c r="AD11" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4851555393243956</v>
+      </c>
+      <c r="AE11" s="1">
+        <f t="shared" si="0"/>
+        <v>13.541766752073968</v>
+      </c>
+      <c r="AF11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.61879601548506</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34">
       <c r="B12" s="103">
         <v>10</v>
       </c>
@@ -33300,8 +36367,51 @@
         <v>6.0659999999999989</v>
       </c>
       <c r="H12" s="99"/>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="T12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dyn1</v>
+      </c>
+      <c r="U12" s="1" cm="1">
+        <f t="array" ref="U12:V12">LINEST(C4:C22,F4:F22)</f>
+        <v>10.262318786991187</v>
+      </c>
+      <c r="V12" s="1">
+        <v>3.7253441448465452</v>
+      </c>
+      <c r="X12" s="1">
+        <f>$D12*$U$10+$V$10</f>
+        <v>124.8676624738676</v>
+      </c>
+      <c r="Y12" s="1">
+        <f>E12*$U$11+$V$11</f>
+        <v>113.37702847352205</v>
+      </c>
+      <c r="Z12" s="1">
+        <f>F12*$U$12+$V$12</f>
+        <v>96.086213227767232</v>
+      </c>
+      <c r="AA12" s="1">
+        <f>G12*$U$13+$V$13</f>
+        <v>81.058969197862965</v>
+      </c>
+      <c r="AC12" s="1">
+        <f t="shared" si="1"/>
+        <v>82.281857595818821</v>
+      </c>
+      <c r="AD12" s="1">
+        <f t="shared" si="0"/>
+        <v>70.791223595473269</v>
+      </c>
+      <c r="AE12" s="1">
+        <f t="shared" si="0"/>
+        <v>53.500408349718448</v>
+      </c>
+      <c r="AF12" s="1">
+        <f t="shared" si="0"/>
+        <v>38.473164319814181</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34">
       <c r="B13" s="103">
         <v>11</v>
       </c>
@@ -33323,8 +36433,51 @@
         <v>4.976</v>
       </c>
       <c r="H13" s="99"/>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="T13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>dyn2</v>
+      </c>
+      <c r="U13" s="1" cm="1">
+        <f t="array" ref="U13:V13">LINEST(C4:C22,G4:G22)</f>
+        <v>19.491774442135785</v>
+      </c>
+      <c r="V13" s="1">
+        <v>-37.178134568132691</v>
+      </c>
+      <c r="X13" s="1">
+        <f>$D13*$U$10+$V$10</f>
+        <v>61.416918832752614</v>
+      </c>
+      <c r="Y13" s="1">
+        <f>E13*$U$11+$V$11</f>
+        <v>61.546197798695374</v>
+      </c>
+      <c r="Z13" s="1">
+        <f>F13*$U$12+$V$12</f>
+        <v>71.456648138988385</v>
+      </c>
+      <c r="AA13" s="1">
+        <f>G13*$U$13+$V$13</f>
+        <v>59.812935055934972</v>
+      </c>
+      <c r="AC13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0568616550522592</v>
+      </c>
+      <c r="AD13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9275826891094994</v>
+      </c>
+      <c r="AE13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9828676511835113</v>
+      </c>
+      <c r="AF13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6608454318699017</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34">
       <c r="B14" s="103">
         <v>12</v>
       </c>
@@ -33346,8 +36499,40 @@
         <v>4.8332000000000006</v>
       </c>
       <c r="H14" s="99"/>
-    </row>
-    <row r="15" spans="2:8">
+      <c r="X14" s="1">
+        <f>$D14*$U$10+$V$10</f>
+        <v>86.797216289198616</v>
+      </c>
+      <c r="Y14" s="1">
+        <f>E14*$U$11+$V$11</f>
+        <v>98.329367955023969</v>
+      </c>
+      <c r="Z14" s="1">
+        <f>F14*$U$12+$V$12</f>
+        <v>61.194329351997197</v>
+      </c>
+      <c r="AA14" s="1">
+        <f>G14*$U$13+$V$13</f>
+        <v>57.029509665597999</v>
+      </c>
+      <c r="AC14" s="1">
+        <f t="shared" si="1"/>
+        <v>26.987191898954705</v>
+      </c>
+      <c r="AD14" s="1">
+        <f t="shared" si="0"/>
+        <v>38.519343564780058</v>
+      </c>
+      <c r="AE14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.384304961753287</v>
+      </c>
+      <c r="AF14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7805147246459114</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34">
       <c r="B15" s="103">
         <v>13</v>
       </c>
@@ -33369,8 +36554,40 @@
         <v>3</v>
       </c>
       <c r="H15" s="99"/>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="X15" s="1">
+        <f>$D15*$U$10+$V$10</f>
+        <v>48.726770104529614</v>
+      </c>
+      <c r="Y15" s="1">
+        <f>E15*$U$11+$V$11</f>
+        <v>53.743707159474155</v>
+      </c>
+      <c r="Z15" s="1">
+        <f>F15*$U$12+$V$12</f>
+        <v>34.512300505820107</v>
+      </c>
+      <c r="AA15" s="1">
+        <f>G15*$U$13+$V$13</f>
+        <v>21.297188758274665</v>
+      </c>
+      <c r="AC15" s="1">
+        <f t="shared" si="1"/>
+        <v>11.30147742160279</v>
+      </c>
+      <c r="AD15" s="1">
+        <f t="shared" si="0"/>
+        <v>16.318414476547332</v>
+      </c>
+      <c r="AE15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.912992177106716</v>
+      </c>
+      <c r="AF15" s="1">
+        <f t="shared" si="0"/>
+        <v>16.128103924652159</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34">
       <c r="B16" s="103">
         <v>14</v>
       </c>
@@ -33392,8 +36609,40 @@
         <v>5.4130162525952006</v>
       </c>
       <c r="H16" s="99"/>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="X16" s="1">
+        <f>$D16*$U$10+$V$10</f>
+        <v>61.416918832752614</v>
+      </c>
+      <c r="Y16" s="1">
+        <f>E16*$U$11+$V$11</f>
+        <v>73.249933757527202</v>
+      </c>
+      <c r="Z16" s="1">
+        <f>F16*$U$12+$V$12</f>
+        <v>54.511507357908535</v>
+      </c>
+      <c r="AA16" s="1">
+        <f>G16*$U$13+$V$13</f>
+        <v>68.331157279068066</v>
+      </c>
+      <c r="AC16" s="1">
+        <f t="shared" si="1"/>
+        <v>13.022211515679452</v>
+      </c>
+      <c r="AD16" s="1">
+        <f t="shared" si="0"/>
+        <v>24.85522644045404</v>
+      </c>
+      <c r="AE16" s="1">
+        <f t="shared" si="0"/>
+        <v>6.116800040835372</v>
+      </c>
+      <c r="AF16" s="1">
+        <f t="shared" si="0"/>
+        <v>19.936449961994903</v>
+      </c>
+    </row>
+    <row r="17" spans="2:32">
       <c r="B17" s="103">
         <v>16</v>
       </c>
@@ -33415,8 +36664,40 @@
         <v>2</v>
       </c>
       <c r="H17" s="99"/>
-    </row>
-    <row r="18" spans="2:8">
+      <c r="X17" s="1">
+        <f>$D17*$U$10+$V$10</f>
+        <v>48.726770104529614</v>
+      </c>
+      <c r="Y17" s="1">
+        <f>E17*$U$11+$V$11</f>
+        <v>51.514424119696656</v>
+      </c>
+      <c r="Z17" s="1">
+        <f>F17*$U$12+$V$12</f>
+        <v>24.24998171882892</v>
+      </c>
+      <c r="AA17" s="1">
+        <f>G17*$U$13+$V$13</f>
+        <v>1.8054143161388794</v>
+      </c>
+      <c r="AC17" s="1">
+        <f t="shared" si="1"/>
+        <v>28.224379860627174</v>
+      </c>
+      <c r="AD17" s="1">
+        <f t="shared" si="0"/>
+        <v>31.012033875794216</v>
+      </c>
+      <c r="AE17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7475914749264803</v>
+      </c>
+      <c r="AF17" s="1">
+        <f t="shared" si="0"/>
+        <v>18.69697592776356</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32">
       <c r="B18" s="103">
         <v>17</v>
       </c>
@@ -33438,8 +36719,40 @@
         <v>7.1000000000000005</v>
       </c>
       <c r="H18" s="99"/>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="X18" s="1">
+        <f>$D18*$U$10+$V$10</f>
+        <v>99.48736501742161</v>
+      </c>
+      <c r="Y18" s="1">
+        <f>E18*$U$11+$V$11</f>
+        <v>110.59042467380016</v>
+      </c>
+      <c r="Z18" s="1">
+        <f>F18*$U$12+$V$12</f>
+        <v>65.299256866793669</v>
+      </c>
+      <c r="AA18" s="1">
+        <f>G18*$U$13+$V$13</f>
+        <v>101.21346397103139</v>
+      </c>
+      <c r="AC18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.50104961672474246</v>
+      </c>
+      <c r="AD18" s="1">
+        <f t="shared" si="0"/>
+        <v>10.602010039653806</v>
+      </c>
+      <c r="AE18" s="1">
+        <f t="shared" si="0"/>
+        <v>34.689157767352683</v>
+      </c>
+      <c r="AF18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2250493368850357</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32">
       <c r="B19" s="103">
         <v>19</v>
       </c>
@@ -33461,8 +36774,40 @@
         <v>8.6915907722453642</v>
       </c>
       <c r="H19" s="99"/>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="X19" s="1">
+        <f>$D19*$U$10+$V$10</f>
+        <v>86.797216289198616</v>
+      </c>
+      <c r="Y19" s="1">
+        <f>E19*$U$11+$V$11</f>
+        <v>139.0137834309632</v>
+      </c>
+      <c r="Z19" s="1">
+        <f>F19*$U$12+$V$12</f>
+        <v>116.08542007985569</v>
+      </c>
+      <c r="AA19" s="1">
+        <f>G19*$U$13+$V$13</f>
+        <v>132.23639230782274</v>
+      </c>
+      <c r="AC19" s="1">
+        <f t="shared" si="1"/>
+        <v>58.442612979094093</v>
+      </c>
+      <c r="AD19" s="1">
+        <f t="shared" si="0"/>
+        <v>6.226045837329508</v>
+      </c>
+      <c r="AE19" s="1">
+        <f t="shared" si="0"/>
+        <v>29.154409188437015</v>
+      </c>
+      <c r="AF19" s="1">
+        <f t="shared" si="0"/>
+        <v>13.003436960469969</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32">
       <c r="B20" s="103">
         <v>20</v>
       </c>
@@ -33484,8 +36829,40 @@
         <v>6.4580000000000011</v>
       </c>
       <c r="H20" s="99"/>
-    </row>
-    <row r="21" spans="2:8">
+      <c r="X20" s="1">
+        <f>$D20*$U$10+$V$10</f>
+        <v>99.48736501742161</v>
+      </c>
+      <c r="Y20" s="1">
+        <f>E20*$U$11+$V$11</f>
+        <v>74.921896037360312</v>
+      </c>
+      <c r="Z20" s="1">
+        <f>F20*$U$12+$V$12</f>
+        <v>81.144277073908071</v>
+      </c>
+      <c r="AA20" s="1">
+        <f>G20*$U$13+$V$13</f>
+        <v>88.699744779180236</v>
+      </c>
+      <c r="AC20" s="1">
+        <f t="shared" si="1"/>
+        <v>18.865535749128924</v>
+      </c>
+      <c r="AD20" s="1">
+        <f t="shared" ref="AD20:AD22" si="3">ABS($C20-Y20)</f>
+        <v>5.6999332309323734</v>
+      </c>
+      <c r="AE20" s="1">
+        <f t="shared" ref="AE20:AE22" si="4">ABS($C20-Z20)</f>
+        <v>0.52244780561538562</v>
+      </c>
+      <c r="AF20" s="1">
+        <f t="shared" ref="AF20:AF22" si="5">ABS($C20-AA20)</f>
+        <v>8.07791551088755</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32">
       <c r="B21" s="103">
         <v>21</v>
       </c>
@@ -33507,8 +36884,40 @@
         <v>6.1128912</v>
       </c>
       <c r="H21" s="102"/>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="X21" s="1">
+        <f>$D21*$U$10+$V$10</f>
+        <v>74.107067560975608</v>
+      </c>
+      <c r="Y21" s="1">
+        <f>E21*$U$11+$V$11</f>
+        <v>85.510990476303391</v>
+      </c>
+      <c r="Z21" s="1">
+        <f>F21*$U$12+$V$12</f>
+        <v>71.702943789876173</v>
+      </c>
+      <c r="AA21" s="1">
+        <f>G21*$U$13+$V$13</f>
+        <v>81.972961891584063</v>
+      </c>
+      <c r="AC21" s="1">
+        <f t="shared" si="1"/>
+        <v>15.832151951219515</v>
+      </c>
+      <c r="AD21" s="1">
+        <f t="shared" si="3"/>
+        <v>4.4282290358917322</v>
+      </c>
+      <c r="AE21" s="1">
+        <f t="shared" si="4"/>
+        <v>18.23627572231895</v>
+      </c>
+      <c r="AF21" s="1">
+        <f t="shared" si="5"/>
+        <v>7.96625762061106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32">
       <c r="B22" s="37">
         <v>23</v>
       </c>
@@ -33530,8 +36939,40 @@
         <v>5.7813413250560011</v>
       </c>
       <c r="H22" s="102"/>
-    </row>
-    <row r="23" spans="2:8">
+      <c r="X22" s="1">
+        <f>$D22*$U$10+$V$10</f>
+        <v>74.107067560975608</v>
+      </c>
+      <c r="Y22" s="1">
+        <f>E22*$U$11+$V$11</f>
+        <v>73.807254517471563</v>
+      </c>
+      <c r="Z22" s="1">
+        <f>F22*$U$12+$V$12</f>
+        <v>71.440228428929203</v>
+      </c>
+      <c r="AA22" s="1">
+        <f>G22*$U$13+$V$13</f>
+        <v>75.510466512857306</v>
+      </c>
+      <c r="AC22" s="1">
+        <f t="shared" si="1"/>
+        <v>19.606360243902451</v>
+      </c>
+      <c r="AD22" s="1">
+        <f t="shared" si="3"/>
+        <v>19.306547200398406</v>
+      </c>
+      <c r="AE22" s="1">
+        <f t="shared" si="4"/>
+        <v>16.939521111856045</v>
+      </c>
+      <c r="AF22" s="1">
+        <f t="shared" si="5"/>
+        <v>21.009759195784149</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32">
       <c r="C23" s="74" t="s">
         <v>326</v>
       </c>
@@ -33552,8 +36993,24 @@
         <v>0.93180506545250352</v>
       </c>
       <c r="H23" s="99"/>
-    </row>
-    <row r="24" spans="2:8" hidden="1">
+      <c r="AC23" s="122">
+        <f>AVERAGE(AC4:AC22)</f>
+        <v>26.770956059050064</v>
+      </c>
+      <c r="AD23" s="122">
+        <f>AVERAGE(AD4:AD22)</f>
+        <v>25.68456665394233</v>
+      </c>
+      <c r="AE23" s="122">
+        <f t="shared" ref="AE23:AF23" si="6">AVERAGE(AE4:AE22)</f>
+        <v>16.263023807354067</v>
+      </c>
+      <c r="AF23" s="122">
+        <f t="shared" si="6"/>
+        <v>13.532561849160183</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" hidden="1">
       <c r="C24" s="74" t="s">
         <v>327</v>
       </c>
@@ -33565,8 +37022,8 @@
       <c r="G24" s="74"/>
       <c r="H24" s="99"/>
     </row>
-    <row r="25" spans="2:8" ht="350" customHeight="1"/>
-    <row r="26" spans="2:8">
+    <row r="25" spans="2:32" ht="350" customHeight="1"/>
+    <row r="26" spans="2:32">
       <c r="B26" s="107" t="s">
         <v>505</v>
       </c>
@@ -33574,7 +37031,7 @@
       <c r="D26" s="107"/>
       <c r="E26" s="107"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:32">
       <c r="B28" s="72" t="s">
         <v>49</v>
       </c>
@@ -33588,7 +37045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:32">
       <c r="B29" s="73">
         <v>1</v>
       </c>
@@ -33602,7 +37059,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:32">
       <c r="B30" s="73">
         <v>2</v>
       </c>
@@ -33616,7 +37073,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:32">
       <c r="B31" s="73">
         <v>3</v>
       </c>
@@ -33630,7 +37087,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:32">
       <c r="B32" s="73">
         <v>4</v>
       </c>
@@ -33935,9 +37392,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B1:G1"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="T9:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -36049,7 +39508,7 @@
   <sheetPr codeName="Feuil64"/>
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:G19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding fMRI Peitek experiment 2021
</commit_message>
<xml_diff>
--- a/dataset-cpx.xlsx
+++ b/dataset-cpx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/these/studies/cpx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A5CBF6-416E-F543-9D1E-75E5B083B173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC44FB9-3002-5B46-BE09-2720134F6BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{E3999CCB-9ED0-3445-84E9-42CD1661CA3C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{E3999CCB-9ED0-3445-84E9-42CD1661CA3C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,22 +19,22 @@
     <sheet name="siegmund2012" sheetId="27" r:id="rId4"/>
     <sheet name="peitek2021" sheetId="71" r:id="rId5"/>
     <sheet name="Synthesis" sheetId="82" r:id="rId6"/>
-    <sheet name="ArrAvg" sheetId="65" state="hidden" r:id="rId7"/>
-    <sheet name="CountSubstr" sheetId="66" state="hidden" r:id="rId8"/>
-    <sheet name="CountVwls" sheetId="67" state="hidden" r:id="rId9"/>
-    <sheet name="DumbSort" sheetId="68" state="hidden" r:id="rId10"/>
-    <sheet name="GrCoDiv" sheetId="69" state="hidden" r:id="rId11"/>
-    <sheet name="hIndex" sheetId="70" state="hidden" r:id="rId12"/>
-    <sheet name="isHur" sheetId="72" state="hidden" r:id="rId13"/>
-    <sheet name="isPalind" sheetId="73" state="hidden" r:id="rId14"/>
-    <sheet name="lgthLastWd" sheetId="74" state="hidden" r:id="rId15"/>
-    <sheet name="binToDec" sheetId="75" state="hidden" r:id="rId16"/>
-    <sheet name="crosSum" sheetId="76" state="hidden" r:id="rId17"/>
-    <sheet name="n!" sheetId="77" state="hidden" r:id="rId18"/>
-    <sheet name="fibonacci" sheetId="78" state="hidden" r:id="rId19"/>
-    <sheet name="power" sheetId="79" state="hidden" r:id="rId20"/>
-    <sheet name="sqrt" sheetId="80" state="hidden" r:id="rId21"/>
-    <sheet name="yesNo" sheetId="81" state="hidden" r:id="rId22"/>
+    <sheet name="ArrAvg" sheetId="65" r:id="rId7"/>
+    <sheet name="CountSubstr" sheetId="66" r:id="rId8"/>
+    <sheet name="CountVwls" sheetId="67" r:id="rId9"/>
+    <sheet name="DumbSort" sheetId="68" r:id="rId10"/>
+    <sheet name="GrCoDiv" sheetId="69" r:id="rId11"/>
+    <sheet name="hIndex" sheetId="70" r:id="rId12"/>
+    <sheet name="isHur" sheetId="72" r:id="rId13"/>
+    <sheet name="isPalind" sheetId="73" r:id="rId14"/>
+    <sheet name="lgthLastWd" sheetId="74" r:id="rId15"/>
+    <sheet name="binToDec" sheetId="75" r:id="rId16"/>
+    <sheet name="crosSum" sheetId="76" r:id="rId17"/>
+    <sheet name="n!" sheetId="77" r:id="rId18"/>
+    <sheet name="fibonacci" sheetId="78" r:id="rId19"/>
+    <sheet name="power" sheetId="79" r:id="rId20"/>
+    <sheet name="sqrt" sheetId="80" r:id="rId21"/>
+    <sheet name="yesNo" sheetId="81" r:id="rId22"/>
     <sheet name="1" sheetId="3" r:id="rId23"/>
     <sheet name="2" sheetId="4" r:id="rId24"/>
     <sheet name="3" sheetId="23" r:id="rId25"/>
@@ -61,14 +61,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Feuil37!$B$7:$C$42</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">siegmund2012!$C$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">siegmund2012!$C$4:$C$22</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">siegmund2012!$G$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">siegmund2012!$G$4:$G$22</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">siegmund2012!$C$3</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">siegmund2012!$C$4:$C$22</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">siegmund2012!$G$3</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">siegmund2012!$G$4:$G$22</definedName>
     <definedName name="xdata1" hidden="1">#REF!</definedName>
     <definedName name="xdata2" hidden="1">#REF!</definedName>
     <definedName name="xdata3" hidden="1">#REF!</definedName>
@@ -158,7 +150,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -180,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="513">
   <si>
     <t>snippet_id</t>
   </si>
@@ -6219,7 +6211,19 @@
     <t>dyn2</t>
   </si>
   <si>
-    <t>Linear regression line</t>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Linear regression line / metric</t>
+  </si>
+  <si>
+    <t>Linear regression line / time</t>
+  </si>
+  <si>
+    <t>Forecasted values</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -6396,7 +6400,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6463,8 +6467,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -6590,11 +6600,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6769,6 +6803,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6814,10 +6854,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -10038,7 +10090,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F39DA6A-E70F-004D-A8E4-455A9706DC17}" type="CELLRANGE">
+                    <a:fld id="{716EA338-3C1F-244E-9D51-C4FE0674D0ED}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10071,7 +10123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51348929-3CE8-904D-8782-246BF01051EB}" type="CELLRANGE">
+                    <a:fld id="{A89309CF-6FC5-AC4C-9E2E-FA1C3DF438A5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10104,7 +10156,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{812BA8D4-10F9-2246-8E72-BC438B869F21}" type="CELLRANGE">
+                    <a:fld id="{EEF37AA2-5B25-5D43-AF81-00A49C933ECA}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10137,7 +10189,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0F3FBDB-20E5-CE41-9CD9-9F6DA2B6A509}" type="CELLRANGE">
+                    <a:fld id="{59F77E5C-D7F7-9A43-8BB7-E26CF2C3A096}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10170,7 +10222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FBD59BC-295E-6A45-A49E-7BFDB16F6541}" type="CELLRANGE">
+                    <a:fld id="{FA9E53E0-1275-FB4A-989B-9E716A5E2C44}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10203,7 +10255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7E10F74-FF33-5F4E-A291-CBF4B32EFF9B}" type="CELLRANGE">
+                    <a:fld id="{C717A692-843D-7741-BD7A-FE10C58E523D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10236,7 +10288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DE4E1CA-077C-C740-A9D1-D4630E9A6A2B}" type="CELLRANGE">
+                    <a:fld id="{150A85E3-7563-074E-8D9F-B0F19A944249}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10269,7 +10321,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E324EC8-9509-9142-A4DF-178DE429EA5A}" type="CELLRANGE">
+                    <a:fld id="{0640945A-ABFB-7D44-86B1-7F3A6F1EB3C0}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10302,7 +10354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A1387D7-EFB1-054E-AACF-929E55FC7FBD}" type="CELLRANGE">
+                    <a:fld id="{3698AF80-6535-D24A-9597-D52D38946EA7}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10335,7 +10387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{847C2912-4AE9-2B4A-8612-651823491E89}" type="CELLRANGE">
+                    <a:fld id="{79E07AE9-D24A-F141-9DDB-B509FF55543A}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10368,7 +10420,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1824833-361C-0043-950A-3A2A1D29199D}" type="CELLRANGE">
+                    <a:fld id="{30E752C9-4F93-C448-ADB4-0A4B7EA88890}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10401,7 +10453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6A36DEE-156F-3C46-8796-44474D28D323}" type="CELLRANGE">
+                    <a:fld id="{D00D42D9-51F8-7E43-9329-29A38E2C0414}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10434,7 +10486,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6279345F-23FB-EC4F-AB0B-E32FA94A3D88}" type="CELLRANGE">
+                    <a:fld id="{D0A7A321-56F6-8D4F-87CA-A8FF48CF9074}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10467,7 +10519,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3084130C-DCF6-F246-B0CC-B0BE97F0A1C5}" type="CELLRANGE">
+                    <a:fld id="{1737EA59-78B8-2F4E-906F-B6BE8A95EFF5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10500,7 +10552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1842C9B-B8B9-3747-A93C-1FD3834DDB66}" type="CELLRANGE">
+                    <a:fld id="{B6F109F0-25FF-4145-88D1-AC600ABC5512}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10533,7 +10585,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DD2E44E-D086-E042-9596-A11826EB5F63}" type="CELLRANGE">
+                    <a:fld id="{BAA2942A-5DF6-7840-B8F4-9599242F271C}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10566,7 +10618,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99165BB0-3594-4840-828C-49DA02FD464F}" type="CELLRANGE">
+                    <a:fld id="{DBC37C18-EC5A-224D-953D-7211BDCC346F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10599,7 +10651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C697E4E9-7030-E847-9A41-B68DA8656610}" type="CELLRANGE">
+                    <a:fld id="{EBA822DF-BAC8-B54B-9A5D-5D219C0C5448}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10632,7 +10684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44DCBF68-1548-F04E-B0E7-EB1A600AFDC0}" type="CELLRANGE">
+                    <a:fld id="{4FED90A4-D7A3-AD45-B36C-BA066BFDA48E}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10665,7 +10717,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A0650A8-834E-2543-AA9A-8673BB3F5FC1}" type="CELLRANGE">
+                    <a:fld id="{271AA26E-BD2A-CB4D-8D79-AE1F2BFB55E9}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10698,7 +10750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93F49A16-9BFA-6547-B498-DA637D6C51CB}" type="CELLRANGE">
+                    <a:fld id="{62E5FAF4-5638-454A-9361-30DD38464D45}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10731,7 +10783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9385C19-D00E-5C46-A844-228595570F8C}" type="CELLRANGE">
+                    <a:fld id="{0C0A1082-9DCA-6E42-A349-405022DC45BA}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10764,7 +10816,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54E06FA0-E2D3-5C4D-AEBD-0F6C3D52159E}" type="CELLRANGE">
+                    <a:fld id="{2E494FA3-0F9C-FE4F-8159-A77B639F5CBD}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -11742,7 +11794,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>siegmund2012!$E$28</c:f>
+              <c:f>siegmund2012!$E$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11804,7 +11856,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>siegmund2012!$C$29:$C$51</c:f>
+              <c:f>siegmund2012!$C$30:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="23"/>
@@ -11882,7 +11934,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>siegmund2012!$E$29:$E$51</c:f>
+              <c:f>siegmund2012!$E$30:$E$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -13544,7 +13596,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>siegmund2012!$D$28</c:f>
+              <c:f>siegmund2012!$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13591,7 +13643,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>siegmund2012!$C$29:$C$51</c:f>
+              <c:f>siegmund2012!$C$30:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="23"/>
@@ -13669,7 +13721,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>siegmund2012!$D$29:$D$51</c:f>
+              <c:f>siegmund2012!$D$30:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -22274,13 +22326,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>336313</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>11759</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>740832</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>47037</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22316,8 +22368,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>776111</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>11760</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>188148</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22346,13 +22398,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>399815</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>30339</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>799630</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>3974630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22382,13 +22434,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>154046</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>33631</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>364537</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>3998148</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22418,13 +22470,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>142287</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>10112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>281046</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>23518</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22454,13 +22506,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>89370</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>492242</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>545630</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>4127499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22489,15 +22541,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>492242</xdr:rowOff>
+      <xdr:colOff>606778</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>504001</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>204612</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>4139259</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>239889</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4151018</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23592,16 +23644,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" s="14"/>
@@ -25092,16 +25144,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
     </row>
     <row r="3" spans="1:10">
       <c r="H3" s="29">
@@ -25607,14 +25659,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
     </row>
     <row r="3" spans="1:8">
       <c r="F3" s="26">
@@ -25977,15 +26029,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
     </row>
     <row r="3" spans="1:9">
       <c r="D3" s="31"/>
@@ -26469,12 +26521,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
     </row>
     <row r="3" spans="1:6">
       <c r="D3" s="26">
@@ -26646,15 +26698,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="76"/>
@@ -26922,15 +26974,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="26">
@@ -27763,13 +27815,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="29">
@@ -28030,13 +28082,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="76"/>
@@ -28329,12 +28381,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
     </row>
     <row r="3" spans="1:6">
       <c r="D3" s="29">
@@ -28564,12 +28616,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
     </row>
     <row r="3" spans="1:6">
       <c r="D3" s="29">
@@ -29150,13 +29202,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="29">
@@ -29429,13 +29481,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="29">
@@ -29980,10 +30032,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="117"/>
+      <c r="B1" s="119"/>
     </row>
     <row r="3" spans="1:5">
       <c r="C3" s="26">
@@ -30139,7 +30191,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScale="137" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30149,12 +30201,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="19">
       <c r="A2" s="20"/>
@@ -30446,14 +30498,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="3" spans="1:8">
       <c r="G3" s="42">
@@ -30994,14 +31046,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="2" spans="1:9" ht="19">
       <c r="A2" s="53"/>
@@ -31614,14 +31666,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="42">
@@ -32118,13 +32170,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:6" s="10" customFormat="1">
       <c r="A2" s="57"/>
@@ -32411,13 +32463,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1"/>
     <row r="3" spans="1:7" s="10" customFormat="1">
@@ -33402,13 +33454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="75"/>
@@ -33688,14 +33740,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1"/>
     <row r="3" spans="1:8" s="10" customFormat="1">
@@ -34205,13 +34257,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="41">
@@ -34390,14 +34442,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1">
       <c r="A2" s="11"/>
@@ -34618,14 +34670,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1">
       <c r="A2" s="13"/>
@@ -34840,13 +34892,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="13"/>
@@ -35024,13 +35076,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="42">
@@ -35378,13 +35430,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="42">
@@ -35507,15 +35559,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="42">
@@ -35737,10 +35789,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B752191-782E-EA48-B322-664FAB9CF9B3}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="B1:AH53"/>
+  <dimension ref="B1:AG54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView topLeftCell="M1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2:AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -35755,27 +35807,41 @@
     <col min="8" max="8" width="10.5" style="1" customWidth="1"/>
     <col min="9" max="18" width="10.83203125" style="1"/>
     <col min="19" max="19" width="4.1640625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="1"/>
+    <col min="20" max="27" width="10.83203125" style="1"/>
+    <col min="28" max="28" width="3.6640625" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="19">
-      <c r="B1" s="106" t="s">
+    <row r="1" spans="2:33" ht="19">
+      <c r="B1" s="108" t="s">
         <v>474</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-    </row>
-    <row r="2" spans="2:34">
-      <c r="T2" s="121" t="s">
-        <v>508</v>
-      </c>
-      <c r="U2" s="121"/>
-      <c r="V2" s="121"/>
-    </row>
-    <row r="3" spans="2:34">
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+    </row>
+    <row r="2" spans="2:33">
+      <c r="T2" s="116" t="s">
+        <v>509</v>
+      </c>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="X2" s="124" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="126"/>
+      <c r="AD2" s="116" t="s">
+        <v>512</v>
+      </c>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="116"/>
+    </row>
+    <row r="3" spans="2:33">
       <c r="B3" s="72" t="s">
         <v>502</v>
       </c>
@@ -35797,55 +35863,52 @@
         <v>dyn2</v>
       </c>
       <c r="H3" s="99"/>
-      <c r="T3" s="1" t="str">
+      <c r="T3" s="73" t="str">
         <f>D3</f>
         <v>sonarqube</v>
       </c>
-      <c r="U3" s="1" cm="1">
+      <c r="U3" s="73" cm="1">
         <f t="array" ref="U3:V3">LINEST(D4:D22,C4:C22)</f>
         <v>2.4558162269338261E-2</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="73">
         <v>0.68727428091925669</v>
       </c>
-      <c r="X3" s="14" t="str">
+      <c r="X3" s="106" t="str">
         <f>D3</f>
         <v>sonarqube</v>
       </c>
-      <c r="Y3" s="14" t="str">
+      <c r="Y3" s="106" t="str">
         <f>E3</f>
         <v>genese_cpx</v>
       </c>
-      <c r="Z3" s="14" t="str">
+      <c r="Z3" s="106" t="str">
         <f>F3</f>
         <v>dyn1</v>
       </c>
-      <c r="AA3" s="14" t="str">
+      <c r="AA3" s="106" t="str">
         <f>G3</f>
         <v>dyn2</v>
       </c>
-      <c r="AC3" s="14" t="str">
+      <c r="AB3" s="107"/>
+      <c r="AD3" s="106" t="str">
         <f>D3</f>
         <v>sonarqube</v>
       </c>
-      <c r="AD3" s="14" t="str">
+      <c r="AE3" s="106" t="str">
         <f>E3</f>
         <v>genese_cpx</v>
       </c>
-      <c r="AE3" s="14" t="str">
+      <c r="AF3" s="106" t="str">
         <f>F3</f>
         <v>dyn1</v>
       </c>
-      <c r="AF3" s="14" t="str">
+      <c r="AG3" s="106" t="str">
         <f>G3</f>
         <v>dyn2</v>
       </c>
-      <c r="AH3" s="1">
-        <f>STDEV(X4:X22)</f>
-        <v>25.675427112967437</v>
-      </c>
-    </row>
-    <row r="4" spans="2:34">
+    </row>
+    <row r="4" spans="2:33">
       <c r="B4" s="37">
         <v>1</v>
       </c>
@@ -35867,51 +35930,51 @@
         <v>4.8948</v>
       </c>
       <c r="H4" s="99"/>
-      <c r="T4" s="1" t="str">
+      <c r="T4" s="73" t="str">
         <f>E3</f>
         <v>genese_cpx</v>
       </c>
-      <c r="U4" s="1" cm="1">
+      <c r="U4" s="73" cm="1">
         <f t="array" ref="U4:V4">LINEST(E4:E22,C4:C22)</f>
         <v>5.5463678990432835E-2</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="73">
         <v>6.7027076730524611</v>
       </c>
-      <c r="X4" s="1">
-        <f>$D4*$U$10+$V$10</f>
+      <c r="X4" s="73">
+        <f t="shared" ref="X4:X22" si="0">$D4*$U$10+$V$10</f>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y4" s="1">
-        <f>E4*$U$11+$V$11</f>
+      <c r="Y4" s="73">
+        <f t="shared" ref="Y4:Y22" si="1">E4*$U$11+$V$11</f>
         <v>58.202273239029132</v>
       </c>
-      <c r="Z4" s="1">
-        <f>F4*$U$12+$V$12</f>
+      <c r="Z4" s="73">
+        <f t="shared" ref="Z4:Z22" si="2">F4*$U$12+$V$12</f>
         <v>51.752996067965306</v>
       </c>
-      <c r="AA4" s="1">
-        <f>G4*$U$13+$V$13</f>
+      <c r="AA4" s="73">
+        <f t="shared" ref="AA4:AA22" si="3">G4*$U$13+$V$13</f>
         <v>58.230202971233552</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AD4" s="73">
         <f>ABS($C4-X4)</f>
         <v>6.5974958013937197</v>
       </c>
-      <c r="AD4" s="1">
-        <f t="shared" ref="AD4:AF19" si="0">ABS($C4-Y4)</f>
+      <c r="AE4" s="73">
+        <f>ABS($C4-Y4)</f>
         <v>9.8121413951172016</v>
       </c>
-      <c r="AE4" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF4" s="73">
+        <f>ABS($C4-Z4)</f>
         <v>16.261418566181028</v>
       </c>
-      <c r="AF4" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG4" s="73">
+        <f>ABS($C4-AA4)</f>
         <v>9.7842116629127815</v>
       </c>
     </row>
-    <row r="5" spans="2:34">
+    <row r="5" spans="2:33">
       <c r="B5" s="37">
         <v>2</v>
       </c>
@@ -35933,51 +35996,51 @@
         <v>7.7837939390651911</v>
       </c>
       <c r="H5" s="99"/>
-      <c r="T5" s="1" t="str">
+      <c r="T5" s="73" t="str">
         <f>F3</f>
         <v>dyn1</v>
       </c>
-      <c r="U5" s="1" cm="1">
+      <c r="U5" s="73" cm="1">
         <f t="array" ref="U5:V5">LINEST(F4:F22,C4:C22)</f>
         <v>7.6128649226312323E-2</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="73">
         <v>1.4159069751836109</v>
       </c>
-      <c r="X5" s="1">
-        <f>$D5*$U$10+$V$10</f>
+      <c r="X5" s="73">
+        <f t="shared" si="0"/>
         <v>112.1775137456446</v>
       </c>
-      <c r="Y5" s="1">
-        <f>E5*$U$11+$V$11</f>
+      <c r="Y5" s="73">
+        <f t="shared" si="1"/>
         <v>121.17951911274326</v>
       </c>
-      <c r="Z5" s="1">
-        <f>F5*$U$12+$V$12</f>
+      <c r="Z5" s="73">
+        <f t="shared" si="2"/>
         <v>113.07798598541521</v>
       </c>
-      <c r="AA5" s="1">
-        <f>G5*$U$13+$V$13</f>
+      <c r="AA5" s="73">
+        <f t="shared" si="3"/>
         <v>114.54182119618963</v>
       </c>
-      <c r="AC5" s="1">
-        <f t="shared" ref="AC5:AC22" si="1">ABS($C5-X5)</f>
+      <c r="AD5" s="73">
+        <f t="shared" ref="AD5:AD22" si="4">ABS($C5-X5)</f>
         <v>11.910099111498283</v>
       </c>
-      <c r="AD5" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE5" s="73">
+        <f>ABS($C5-Y5)</f>
         <v>20.912104478596945</v>
       </c>
-      <c r="AE5" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF5" s="73">
+        <f>ABS($C5-Z5)</f>
         <v>12.810571351268891</v>
       </c>
-      <c r="AF5" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG5" s="73">
+        <f>ABS($C5-AA5)</f>
         <v>14.27440656204331</v>
       </c>
     </row>
-    <row r="6" spans="2:34">
+    <row r="6" spans="2:33">
       <c r="B6" s="37">
         <v>4</v>
       </c>
@@ -35999,51 +36062,51 @@
         <v>9.3121798400000007</v>
       </c>
       <c r="H6" s="99"/>
-      <c r="T6" s="1" t="str">
+      <c r="T6" s="73" t="str">
         <f>G3</f>
         <v>dyn2</v>
       </c>
-      <c r="U6" s="1" cm="1">
+      <c r="U6" s="73" cm="1">
         <f t="array" ref="U6:V6">LINEST(G4:G22,C4:C22)</f>
         <v>4.4544978836098509E-2</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="73">
         <v>2.4714422904012738</v>
       </c>
-      <c r="X6" s="1">
-        <f>$D6*$U$10+$V$10</f>
+      <c r="X6" s="73">
+        <f t="shared" si="0"/>
         <v>137.55781120209062</v>
       </c>
-      <c r="Y6" s="1">
-        <f>E6*$U$11+$V$11</f>
+      <c r="Y6" s="73">
+        <f t="shared" si="1"/>
         <v>106.13185859424519</v>
       </c>
-      <c r="Z6" s="1">
-        <f>F6*$U$12+$V$12</f>
+      <c r="Z6" s="73">
+        <f t="shared" si="2"/>
         <v>162.09344766569455</v>
       </c>
-      <c r="AA6" s="1">
-        <f>G6*$U$13+$V$13</f>
+      <c r="AA6" s="73">
+        <f t="shared" si="3"/>
         <v>144.33277443775143</v>
       </c>
-      <c r="AC6" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD6" s="73">
+        <f t="shared" si="4"/>
         <v>17.083749773519173</v>
       </c>
-      <c r="AD6" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE6" s="73">
+        <f>ABS($C6-Y6)</f>
         <v>48.509702381364605</v>
       </c>
-      <c r="AE6" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF6" s="73">
+        <f>ABS($C6-Z6)</f>
         <v>7.4518866900847627</v>
       </c>
-      <c r="AF6" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG6" s="73">
+        <f>ABS($C6-AA6)</f>
         <v>10.308786537858367</v>
       </c>
     </row>
-    <row r="7" spans="2:34">
+    <row r="7" spans="2:33">
       <c r="B7" s="37">
         <v>5</v>
       </c>
@@ -36065,40 +36128,40 @@
         <v>11.704923999999998</v>
       </c>
       <c r="H7" s="99"/>
-      <c r="X7" s="1">
-        <f>$D7*$U$10+$V$10</f>
+      <c r="X7" s="73">
+        <f t="shared" si="0"/>
         <v>112.1775137456446</v>
       </c>
-      <c r="Y7" s="1">
-        <f>E7*$U$11+$V$11</f>
+      <c r="Y7" s="73">
+        <f t="shared" si="1"/>
         <v>100.00133023485711</v>
       </c>
-      <c r="Z7" s="1">
-        <f>F7*$U$12+$V$12</f>
+      <c r="Z7" s="73">
+        <f t="shared" si="2"/>
         <v>189.67856056512687</v>
       </c>
-      <c r="AA7" s="1">
-        <f>G7*$U$13+$V$13</f>
+      <c r="AA7" s="73">
+        <f t="shared" si="3"/>
         <v>190.97160390220904</v>
       </c>
-      <c r="AC7" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD7" s="73">
+        <f t="shared" si="4"/>
         <v>99.307022839721242</v>
       </c>
-      <c r="AD7" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE7" s="73">
+        <f>ABS($C7-Y7)</f>
         <v>111.48320635050874</v>
       </c>
-      <c r="AE7" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF7" s="73">
+        <f>ABS($C7-Z7)</f>
         <v>21.805976020238973</v>
       </c>
-      <c r="AF7" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG7" s="73">
+        <f>ABS($C7-AA7)</f>
         <v>20.512932683156805</v>
       </c>
     </row>
-    <row r="8" spans="2:34">
+    <row r="8" spans="2:33">
       <c r="B8" s="37">
         <v>6</v>
       </c>
@@ -36120,40 +36183,40 @@
         <v>4.7900520000000002</v>
       </c>
       <c r="H8" s="99"/>
-      <c r="X8" s="1">
-        <f>$D8*$U$10+$V$10</f>
+      <c r="X8" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y8" s="1">
-        <f>E8*$U$11+$V$11</f>
+      <c r="Y8" s="73">
+        <f t="shared" si="1"/>
         <v>59.87423551886225</v>
       </c>
-      <c r="Z8" s="1">
-        <f>F8*$U$12+$V$12</f>
+      <c r="Z8" s="73">
+        <f t="shared" si="2"/>
         <v>53.723361275067617</v>
       </c>
-      <c r="AA8" s="1">
-        <f>G8*$U$13+$V$13</f>
+      <c r="AA8" s="73">
+        <f t="shared" si="3"/>
         <v>56.18847858196871</v>
       </c>
-      <c r="AC8" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD8" s="73">
+        <f t="shared" si="4"/>
         <v>9.0940323867595652</v>
       </c>
-      <c r="AD8" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE8" s="73">
+        <f>ABS($C8-Y8)</f>
         <v>10.63671570064993</v>
       </c>
-      <c r="AE8" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF8" s="73">
+        <f>ABS($C8-Z8)</f>
         <v>16.787589944444562</v>
       </c>
-      <c r="AF8" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG8" s="73">
+        <f>ABS($C8-AA8)</f>
         <v>14.32247263754347</v>
       </c>
     </row>
-    <row r="9" spans="2:34">
+    <row r="9" spans="2:33">
       <c r="B9" s="37">
         <v>7</v>
       </c>
@@ -36175,45 +36238,45 @@
         <v>6.6073685280000003</v>
       </c>
       <c r="H9" s="99"/>
-      <c r="T9" s="121" t="s">
-        <v>508</v>
-      </c>
-      <c r="U9" s="121"/>
-      <c r="V9" s="121"/>
-      <c r="X9" s="1">
-        <f>$D9*$U$10+$V$10</f>
+      <c r="T9" s="116" t="s">
+        <v>510</v>
+      </c>
+      <c r="U9" s="116"/>
+      <c r="V9" s="116"/>
+      <c r="X9" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y9" s="1">
-        <f>E9*$U$11+$V$11</f>
+      <c r="Y9" s="73">
+        <f t="shared" si="1"/>
         <v>73.249933757527202</v>
       </c>
-      <c r="Z9" s="1">
-        <f>F9*$U$12+$V$12</f>
+      <c r="Z9" s="73">
+        <f t="shared" si="2"/>
         <v>98.54916973664514</v>
       </c>
-      <c r="AA9" s="1">
-        <f>G9*$U$13+$V$13</f>
+      <c r="AA9" s="73">
+        <f t="shared" si="3"/>
         <v>91.611202435710055</v>
       </c>
-      <c r="AC9" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD9" s="73">
+        <f t="shared" si="4"/>
         <v>20.748606533101082</v>
       </c>
-      <c r="AD9" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE9" s="73">
+        <f>ABS($C9-Y9)</f>
         <v>7.2013240014296684</v>
       </c>
-      <c r="AE9" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF9" s="73">
+        <f>ABS($C9-Z9)</f>
         <v>32.500559980547607</v>
       </c>
-      <c r="AF9" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG9" s="73">
+        <f>ABS($C9-AA9)</f>
         <v>25.562592679612521</v>
       </c>
     </row>
-    <row r="10" spans="2:34">
+    <row r="10" spans="2:33">
       <c r="B10" s="103">
         <v>8</v>
       </c>
@@ -36235,51 +36298,51 @@
         <v>6.8864000000000001</v>
       </c>
       <c r="H10" s="99"/>
-      <c r="T10" s="1" t="str">
+      <c r="T10" s="73" t="str">
         <f>T3</f>
         <v>sonarqube</v>
       </c>
-      <c r="U10" s="1" cm="1">
+      <c r="U10" s="73" cm="1">
         <f t="array" ref="U10:V10">LINEST(C4:C22,D4:D22)</f>
         <v>12.690148728222999</v>
       </c>
-      <c r="V10" s="1">
+      <c r="V10" s="73">
         <v>48.726770104529614</v>
       </c>
-      <c r="X10" s="1">
-        <f>$D10*$U$10+$V$10</f>
+      <c r="X10" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y10" s="1">
-        <f>E10*$U$11+$V$11</f>
+      <c r="Y10" s="73">
+        <f t="shared" si="1"/>
         <v>61.546197798695374</v>
       </c>
-      <c r="Z10" s="1">
-        <f>F10*$U$12+$V$12</f>
+      <c r="Z10" s="73">
+        <f t="shared" si="2"/>
         <v>90.175117606460319</v>
       </c>
-      <c r="AA10" s="1">
-        <f>G10*$U$13+$V$13</f>
+      <c r="AA10" s="73">
+        <f t="shared" si="3"/>
         <v>97.050020950191168</v>
       </c>
-      <c r="AC10" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD10" s="73">
+        <f t="shared" si="4"/>
         <v>43.409105557491316</v>
       </c>
-      <c r="AD10" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE10" s="73">
+        <f>ABS($C10-Y10)</f>
         <v>43.279826591548556</v>
       </c>
-      <c r="AE10" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF10" s="73">
+        <f>ABS($C10-Z10)</f>
         <v>14.650906783783611</v>
       </c>
-      <c r="AF10" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG10" s="73">
+        <f>ABS($C10-AA10)</f>
         <v>7.7760034400527616</v>
       </c>
     </row>
-    <row r="11" spans="2:34">
+    <row r="11" spans="2:33">
       <c r="B11" s="103">
         <v>9</v>
       </c>
@@ -36301,51 +36364,51 @@
         <v>5.1806567180919743</v>
       </c>
       <c r="H11" s="99"/>
-      <c r="T11" s="1" t="str">
-        <f t="shared" ref="T11:T13" si="2">T4</f>
+      <c r="T11" s="73" t="str">
+        <f t="shared" ref="T11:T13" si="5">T4</f>
         <v>genese_cpx</v>
       </c>
-      <c r="U11" s="1" cm="1">
+      <c r="U11" s="73" cm="1">
         <f t="array" ref="U11:V11">LINEST(C4:C22,E4:E22)</f>
         <v>5.5732075994437276</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V11" s="73">
         <v>20.304461562811788</v>
       </c>
-      <c r="X11" s="1">
-        <f>$D11*$U$10+$V$10</f>
+      <c r="X11" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y11" s="1">
-        <f>E11*$U$11+$V$11</f>
+      <c r="Y11" s="73">
+        <f t="shared" si="1"/>
         <v>69.906009197860968</v>
       </c>
-      <c r="Z11" s="1">
-        <f>F11*$U$12+$V$12</f>
+      <c r="Z11" s="73">
+        <f t="shared" si="2"/>
         <v>78.96262041061054</v>
       </c>
-      <c r="AA11" s="1">
-        <f>G11*$U$13+$V$13</f>
+      <c r="AA11" s="73">
+        <f t="shared" si="3"/>
         <v>63.802057643051512</v>
       </c>
-      <c r="AC11" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD11" s="73">
+        <f t="shared" si="4"/>
         <v>21.376362630662044</v>
       </c>
-      <c r="AD11" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE11" s="73">
+        <f>ABS($C11-Y11)</f>
         <v>4.4851555393243956</v>
       </c>
-      <c r="AE11" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF11" s="73">
+        <f>ABS($C11-Z11)</f>
         <v>13.541766752073968</v>
       </c>
-      <c r="AF11" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG11" s="73">
+        <f>ABS($C11-AA11)</f>
         <v>1.61879601548506</v>
       </c>
     </row>
-    <row r="12" spans="2:34">
+    <row r="12" spans="2:33">
       <c r="B12" s="103">
         <v>10</v>
       </c>
@@ -36367,51 +36430,51 @@
         <v>6.0659999999999989</v>
       </c>
       <c r="H12" s="99"/>
-      <c r="T12" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="T12" s="73" t="str">
+        <f t="shared" si="5"/>
         <v>dyn1</v>
       </c>
-      <c r="U12" s="1" cm="1">
+      <c r="U12" s="73" cm="1">
         <f t="array" ref="U12:V12">LINEST(C4:C22,F4:F22)</f>
         <v>10.262318786991187</v>
       </c>
-      <c r="V12" s="1">
+      <c r="V12" s="73">
         <v>3.7253441448465452</v>
       </c>
-      <c r="X12" s="1">
-        <f>$D12*$U$10+$V$10</f>
+      <c r="X12" s="73">
+        <f t="shared" si="0"/>
         <v>124.8676624738676</v>
       </c>
-      <c r="Y12" s="1">
-        <f>E12*$U$11+$V$11</f>
+      <c r="Y12" s="73">
+        <f t="shared" si="1"/>
         <v>113.37702847352205</v>
       </c>
-      <c r="Z12" s="1">
-        <f>F12*$U$12+$V$12</f>
+      <c r="Z12" s="73">
+        <f t="shared" si="2"/>
         <v>96.086213227767232</v>
       </c>
-      <c r="AA12" s="1">
-        <f>G12*$U$13+$V$13</f>
+      <c r="AA12" s="73">
+        <f t="shared" si="3"/>
         <v>81.058969197862965</v>
       </c>
-      <c r="AC12" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD12" s="73">
+        <f t="shared" si="4"/>
         <v>82.281857595818821</v>
       </c>
-      <c r="AD12" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE12" s="73">
+        <f>ABS($C12-Y12)</f>
         <v>70.791223595473269</v>
       </c>
-      <c r="AE12" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF12" s="73">
+        <f>ABS($C12-Z12)</f>
         <v>53.500408349718448</v>
       </c>
-      <c r="AF12" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG12" s="73">
+        <f>ABS($C12-AA12)</f>
         <v>38.473164319814181</v>
       </c>
     </row>
-    <row r="13" spans="2:34">
+    <row r="13" spans="2:33">
       <c r="B13" s="103">
         <v>11</v>
       </c>
@@ -36433,51 +36496,51 @@
         <v>4.976</v>
       </c>
       <c r="H13" s="99"/>
-      <c r="T13" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="T13" s="73" t="str">
+        <f t="shared" si="5"/>
         <v>dyn2</v>
       </c>
-      <c r="U13" s="1" cm="1">
+      <c r="U13" s="73" cm="1">
         <f t="array" ref="U13:V13">LINEST(C4:C22,G4:G22)</f>
         <v>19.491774442135785</v>
       </c>
-      <c r="V13" s="1">
+      <c r="V13" s="73">
         <v>-37.178134568132691</v>
       </c>
-      <c r="X13" s="1">
-        <f>$D13*$U$10+$V$10</f>
+      <c r="X13" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y13" s="1">
-        <f>E13*$U$11+$V$11</f>
+      <c r="Y13" s="73">
+        <f t="shared" si="1"/>
         <v>61.546197798695374</v>
       </c>
-      <c r="Z13" s="1">
-        <f>F13*$U$12+$V$12</f>
+      <c r="Z13" s="73">
+        <f t="shared" si="2"/>
         <v>71.456648138988385</v>
       </c>
-      <c r="AA13" s="1">
-        <f>G13*$U$13+$V$13</f>
+      <c r="AA13" s="73">
+        <f t="shared" si="3"/>
         <v>59.812935055934972</v>
       </c>
-      <c r="AC13" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD13" s="73">
+        <f t="shared" si="4"/>
         <v>4.0568616550522592</v>
       </c>
-      <c r="AD13" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE13" s="73">
+        <f>ABS($C13-Y13)</f>
         <v>3.9275826891094994</v>
       </c>
-      <c r="AE13" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF13" s="73">
+        <f>ABS($C13-Z13)</f>
         <v>5.9828676511835113</v>
       </c>
-      <c r="AF13" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG13" s="73">
+        <f>ABS($C13-AA13)</f>
         <v>5.6608454318699017</v>
       </c>
     </row>
-    <row r="14" spans="2:34">
+    <row r="14" spans="2:33">
       <c r="B14" s="103">
         <v>12</v>
       </c>
@@ -36499,40 +36562,40 @@
         <v>4.8332000000000006</v>
       </c>
       <c r="H14" s="99"/>
-      <c r="X14" s="1">
-        <f>$D14*$U$10+$V$10</f>
+      <c r="X14" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y14" s="1">
-        <f>E14*$U$11+$V$11</f>
+      <c r="Y14" s="73">
+        <f t="shared" si="1"/>
         <v>98.329367955023969</v>
       </c>
-      <c r="Z14" s="1">
-        <f>F14*$U$12+$V$12</f>
+      <c r="Z14" s="73">
+        <f t="shared" si="2"/>
         <v>61.194329351997197</v>
       </c>
-      <c r="AA14" s="1">
-        <f>G14*$U$13+$V$13</f>
+      <c r="AA14" s="73">
+        <f t="shared" si="3"/>
         <v>57.029509665597999</v>
       </c>
-      <c r="AC14" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD14" s="73">
+        <f t="shared" si="4"/>
         <v>26.987191898954705</v>
       </c>
-      <c r="AD14" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE14" s="73">
+        <f>ABS($C14-Y14)</f>
         <v>38.519343564780058</v>
       </c>
-      <c r="AE14" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF14" s="73">
+        <f>ABS($C14-Z14)</f>
         <v>1.384304961753287</v>
       </c>
-      <c r="AF14" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG14" s="73">
+        <f>ABS($C14-AA14)</f>
         <v>2.7805147246459114</v>
       </c>
     </row>
-    <row r="15" spans="2:34">
+    <row r="15" spans="2:33">
       <c r="B15" s="103">
         <v>13</v>
       </c>
@@ -36554,40 +36617,40 @@
         <v>3</v>
       </c>
       <c r="H15" s="99"/>
-      <c r="X15" s="1">
-        <f>$D15*$U$10+$V$10</f>
+      <c r="X15" s="73">
+        <f t="shared" si="0"/>
         <v>48.726770104529614</v>
       </c>
-      <c r="Y15" s="1">
-        <f>E15*$U$11+$V$11</f>
+      <c r="Y15" s="73">
+        <f t="shared" si="1"/>
         <v>53.743707159474155</v>
       </c>
-      <c r="Z15" s="1">
-        <f>F15*$U$12+$V$12</f>
+      <c r="Z15" s="73">
+        <f t="shared" si="2"/>
         <v>34.512300505820107</v>
       </c>
-      <c r="AA15" s="1">
-        <f>G15*$U$13+$V$13</f>
+      <c r="AA15" s="73">
+        <f t="shared" si="3"/>
         <v>21.297188758274665</v>
       </c>
-      <c r="AC15" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD15" s="73">
+        <f t="shared" si="4"/>
         <v>11.30147742160279</v>
       </c>
-      <c r="AD15" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE15" s="73">
+        <f>ABS($C15-Y15)</f>
         <v>16.318414476547332</v>
       </c>
-      <c r="AE15" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF15" s="73">
+        <f>ABS($C15-Z15)</f>
         <v>2.912992177106716</v>
       </c>
-      <c r="AF15" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG15" s="73">
+        <f>ABS($C15-AA15)</f>
         <v>16.128103924652159</v>
       </c>
     </row>
-    <row r="16" spans="2:34">
+    <row r="16" spans="2:33">
       <c r="B16" s="103">
         <v>14</v>
       </c>
@@ -36609,40 +36672,40 @@
         <v>5.4130162525952006</v>
       </c>
       <c r="H16" s="99"/>
-      <c r="X16" s="1">
-        <f>$D16*$U$10+$V$10</f>
+      <c r="X16" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y16" s="1">
-        <f>E16*$U$11+$V$11</f>
+      <c r="Y16" s="73">
+        <f t="shared" si="1"/>
         <v>73.249933757527202</v>
       </c>
-      <c r="Z16" s="1">
-        <f>F16*$U$12+$V$12</f>
+      <c r="Z16" s="73">
+        <f t="shared" si="2"/>
         <v>54.511507357908535</v>
       </c>
-      <c r="AA16" s="1">
-        <f>G16*$U$13+$V$13</f>
+      <c r="AA16" s="73">
+        <f t="shared" si="3"/>
         <v>68.331157279068066</v>
       </c>
-      <c r="AC16" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD16" s="73">
+        <f t="shared" si="4"/>
         <v>13.022211515679452</v>
       </c>
-      <c r="AD16" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE16" s="73">
+        <f>ABS($C16-Y16)</f>
         <v>24.85522644045404</v>
       </c>
-      <c r="AE16" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF16" s="73">
+        <f>ABS($C16-Z16)</f>
         <v>6.116800040835372</v>
       </c>
-      <c r="AF16" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG16" s="73">
+        <f>ABS($C16-AA16)</f>
         <v>19.936449961994903</v>
       </c>
     </row>
-    <row r="17" spans="2:32">
+    <row r="17" spans="2:33">
       <c r="B17" s="103">
         <v>16</v>
       </c>
@@ -36664,40 +36727,40 @@
         <v>2</v>
       </c>
       <c r="H17" s="99"/>
-      <c r="X17" s="1">
-        <f>$D17*$U$10+$V$10</f>
+      <c r="X17" s="73">
+        <f t="shared" si="0"/>
         <v>48.726770104529614</v>
       </c>
-      <c r="Y17" s="1">
-        <f>E17*$U$11+$V$11</f>
+      <c r="Y17" s="73">
+        <f t="shared" si="1"/>
         <v>51.514424119696656</v>
       </c>
-      <c r="Z17" s="1">
-        <f>F17*$U$12+$V$12</f>
+      <c r="Z17" s="73">
+        <f t="shared" si="2"/>
         <v>24.24998171882892</v>
       </c>
-      <c r="AA17" s="1">
-        <f>G17*$U$13+$V$13</f>
+      <c r="AA17" s="73">
+        <f t="shared" si="3"/>
         <v>1.8054143161388794</v>
       </c>
-      <c r="AC17" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD17" s="73">
+        <f t="shared" si="4"/>
         <v>28.224379860627174</v>
       </c>
-      <c r="AD17" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE17" s="73">
+        <f>ABS($C17-Y17)</f>
         <v>31.012033875794216</v>
       </c>
-      <c r="AE17" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF17" s="73">
+        <f>ABS($C17-Z17)</f>
         <v>3.7475914749264803</v>
       </c>
-      <c r="AF17" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG17" s="73">
+        <f>ABS($C17-AA17)</f>
         <v>18.69697592776356</v>
       </c>
     </row>
-    <row r="18" spans="2:32">
+    <row r="18" spans="2:33">
       <c r="B18" s="103">
         <v>17</v>
       </c>
@@ -36719,40 +36782,40 @@
         <v>7.1000000000000005</v>
       </c>
       <c r="H18" s="99"/>
-      <c r="X18" s="1">
-        <f>$D18*$U$10+$V$10</f>
+      <c r="X18" s="73">
+        <f t="shared" si="0"/>
         <v>99.48736501742161</v>
       </c>
-      <c r="Y18" s="1">
-        <f>E18*$U$11+$V$11</f>
+      <c r="Y18" s="73">
+        <f t="shared" si="1"/>
         <v>110.59042467380016</v>
       </c>
-      <c r="Z18" s="1">
-        <f>F18*$U$12+$V$12</f>
+      <c r="Z18" s="73">
+        <f t="shared" si="2"/>
         <v>65.299256866793669</v>
       </c>
-      <c r="AA18" s="1">
-        <f>G18*$U$13+$V$13</f>
+      <c r="AA18" s="73">
+        <f t="shared" si="3"/>
         <v>101.21346397103139</v>
       </c>
-      <c r="AC18" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD18" s="73">
+        <f t="shared" si="4"/>
         <v>0.50104961672474246</v>
       </c>
-      <c r="AD18" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE18" s="73">
+        <f>ABS($C18-Y18)</f>
         <v>10.602010039653806</v>
       </c>
-      <c r="AE18" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF18" s="73">
+        <f>ABS($C18-Z18)</f>
         <v>34.689157767352683</v>
       </c>
-      <c r="AF18" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG18" s="73">
+        <f>ABS($C18-AA18)</f>
         <v>1.2250493368850357</v>
       </c>
     </row>
-    <row r="19" spans="2:32">
+    <row r="19" spans="2:33">
       <c r="B19" s="103">
         <v>19</v>
       </c>
@@ -36774,40 +36837,40 @@
         <v>8.6915907722453642</v>
       </c>
       <c r="H19" s="99"/>
-      <c r="X19" s="1">
-        <f>$D19*$U$10+$V$10</f>
+      <c r="X19" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y19" s="1">
-        <f>E19*$U$11+$V$11</f>
+      <c r="Y19" s="73">
+        <f t="shared" si="1"/>
         <v>139.0137834309632</v>
       </c>
-      <c r="Z19" s="1">
-        <f>F19*$U$12+$V$12</f>
+      <c r="Z19" s="73">
+        <f t="shared" si="2"/>
         <v>116.08542007985569</v>
       </c>
-      <c r="AA19" s="1">
-        <f>G19*$U$13+$V$13</f>
+      <c r="AA19" s="73">
+        <f t="shared" si="3"/>
         <v>132.23639230782274</v>
       </c>
-      <c r="AC19" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD19" s="73">
+        <f t="shared" si="4"/>
         <v>58.442612979094093</v>
       </c>
-      <c r="AD19" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE19" s="73">
+        <f>ABS($C19-Y19)</f>
         <v>6.226045837329508</v>
       </c>
-      <c r="AE19" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF19" s="73">
+        <f>ABS($C19-Z19)</f>
         <v>29.154409188437015</v>
       </c>
-      <c r="AF19" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG19" s="73">
+        <f>ABS($C19-AA19)</f>
         <v>13.003436960469969</v>
       </c>
     </row>
-    <row r="20" spans="2:32">
+    <row r="20" spans="2:33">
       <c r="B20" s="103">
         <v>20</v>
       </c>
@@ -36829,40 +36892,40 @@
         <v>6.4580000000000011</v>
       </c>
       <c r="H20" s="99"/>
-      <c r="X20" s="1">
-        <f>$D20*$U$10+$V$10</f>
+      <c r="X20" s="73">
+        <f t="shared" si="0"/>
         <v>99.48736501742161</v>
       </c>
-      <c r="Y20" s="1">
-        <f>E20*$U$11+$V$11</f>
+      <c r="Y20" s="73">
+        <f t="shared" si="1"/>
         <v>74.921896037360312</v>
       </c>
-      <c r="Z20" s="1">
-        <f>F20*$U$12+$V$12</f>
+      <c r="Z20" s="73">
+        <f t="shared" si="2"/>
         <v>81.144277073908071</v>
       </c>
-      <c r="AA20" s="1">
-        <f>G20*$U$13+$V$13</f>
+      <c r="AA20" s="73">
+        <f t="shared" si="3"/>
         <v>88.699744779180236</v>
       </c>
-      <c r="AC20" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD20" s="73">
+        <f t="shared" si="4"/>
         <v>18.865535749128924</v>
       </c>
-      <c r="AD20" s="1">
-        <f t="shared" ref="AD20:AD22" si="3">ABS($C20-Y20)</f>
+      <c r="AE20" s="73">
+        <f t="shared" ref="AE20:AE22" si="6">ABS($C20-Y20)</f>
         <v>5.6999332309323734</v>
       </c>
-      <c r="AE20" s="1">
-        <f t="shared" ref="AE20:AE22" si="4">ABS($C20-Z20)</f>
+      <c r="AF20" s="73">
+        <f t="shared" ref="AF20:AF22" si="7">ABS($C20-Z20)</f>
         <v>0.52244780561538562</v>
       </c>
-      <c r="AF20" s="1">
-        <f t="shared" ref="AF20:AF22" si="5">ABS($C20-AA20)</f>
+      <c r="AG20" s="73">
+        <f t="shared" ref="AG20:AG22" si="8">ABS($C20-AA20)</f>
         <v>8.07791551088755</v>
       </c>
     </row>
-    <row r="21" spans="2:32">
+    <row r="21" spans="2:33">
       <c r="B21" s="103">
         <v>21</v>
       </c>
@@ -36884,40 +36947,40 @@
         <v>6.1128912</v>
       </c>
       <c r="H21" s="102"/>
-      <c r="X21" s="1">
-        <f>$D21*$U$10+$V$10</f>
+      <c r="X21" s="73">
+        <f t="shared" si="0"/>
         <v>74.107067560975608</v>
       </c>
-      <c r="Y21" s="1">
-        <f>E21*$U$11+$V$11</f>
+      <c r="Y21" s="73">
+        <f t="shared" si="1"/>
         <v>85.510990476303391</v>
       </c>
-      <c r="Z21" s="1">
-        <f>F21*$U$12+$V$12</f>
+      <c r="Z21" s="73">
+        <f t="shared" si="2"/>
         <v>71.702943789876173</v>
       </c>
-      <c r="AA21" s="1">
-        <f>G21*$U$13+$V$13</f>
+      <c r="AA21" s="73">
+        <f t="shared" si="3"/>
         <v>81.972961891584063</v>
       </c>
-      <c r="AC21" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD21" s="73">
+        <f t="shared" si="4"/>
         <v>15.832151951219515</v>
       </c>
-      <c r="AD21" s="1">
-        <f t="shared" si="3"/>
+      <c r="AE21" s="73">
+        <f t="shared" si="6"/>
         <v>4.4282290358917322</v>
       </c>
-      <c r="AE21" s="1">
-        <f t="shared" si="4"/>
+      <c r="AF21" s="73">
+        <f t="shared" si="7"/>
         <v>18.23627572231895</v>
       </c>
-      <c r="AF21" s="1">
-        <f t="shared" si="5"/>
+      <c r="AG21" s="73">
+        <f t="shared" si="8"/>
         <v>7.96625762061106</v>
       </c>
     </row>
-    <row r="22" spans="2:32">
+    <row r="22" spans="2:33">
       <c r="B22" s="37">
         <v>23</v>
       </c>
@@ -36939,40 +37002,40 @@
         <v>5.7813413250560011</v>
       </c>
       <c r="H22" s="102"/>
-      <c r="X22" s="1">
-        <f>$D22*$U$10+$V$10</f>
+      <c r="X22" s="73">
+        <f t="shared" si="0"/>
         <v>74.107067560975608</v>
       </c>
-      <c r="Y22" s="1">
-        <f>E22*$U$11+$V$11</f>
+      <c r="Y22" s="73">
+        <f t="shared" si="1"/>
         <v>73.807254517471563</v>
       </c>
-      <c r="Z22" s="1">
-        <f>F22*$U$12+$V$12</f>
+      <c r="Z22" s="73">
+        <f t="shared" si="2"/>
         <v>71.440228428929203</v>
       </c>
-      <c r="AA22" s="1">
-        <f>G22*$U$13+$V$13</f>
+      <c r="AA22" s="73">
+        <f t="shared" si="3"/>
         <v>75.510466512857306</v>
       </c>
-      <c r="AC22" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD22" s="73">
+        <f t="shared" si="4"/>
         <v>19.606360243902451</v>
       </c>
-      <c r="AD22" s="1">
-        <f t="shared" si="3"/>
+      <c r="AE22" s="73">
+        <f t="shared" si="6"/>
         <v>19.306547200398406</v>
       </c>
-      <c r="AE22" s="1">
-        <f t="shared" si="4"/>
+      <c r="AF22" s="73">
+        <f t="shared" si="7"/>
         <v>16.939521111856045</v>
       </c>
-      <c r="AF22" s="1">
-        <f t="shared" si="5"/>
+      <c r="AG22" s="73">
+        <f t="shared" si="8"/>
         <v>21.009759195784149</v>
       </c>
     </row>
-    <row r="23" spans="2:32">
+    <row r="23" spans="2:33">
       <c r="C23" s="74" t="s">
         <v>326</v>
       </c>
@@ -36993,24 +37056,27 @@
         <v>0.93180506545250352</v>
       </c>
       <c r="H23" s="99"/>
-      <c r="AC23" s="122">
-        <f>AVERAGE(AC4:AC22)</f>
+      <c r="AC23" s="127" t="s">
+        <v>483</v>
+      </c>
+      <c r="AD23" s="127">
+        <f>AVERAGE(AD4:AD22)</f>
         <v>26.770956059050064</v>
       </c>
-      <c r="AD23" s="122">
-        <f>AVERAGE(AD4:AD22)</f>
+      <c r="AE23" s="127">
+        <f>AVERAGE(AE4:AE22)</f>
         <v>25.68456665394233</v>
       </c>
-      <c r="AE23" s="122">
-        <f t="shared" ref="AE23:AF23" si="6">AVERAGE(AE4:AE22)</f>
+      <c r="AF23" s="127">
+        <f t="shared" ref="AF23:AG23" si="9">AVERAGE(AF4:AF22)</f>
         <v>16.263023807354067</v>
       </c>
-      <c r="AF23" s="122">
-        <f t="shared" si="6"/>
+      <c r="AG23" s="127">
+        <f t="shared" si="9"/>
         <v>13.532561849160183</v>
       </c>
     </row>
-    <row r="24" spans="2:32" hidden="1">
+    <row r="24" spans="2:33" hidden="1">
       <c r="C24" s="74" t="s">
         <v>327</v>
       </c>
@@ -37021,382 +37087,416 @@
       </c>
       <c r="G24" s="74"/>
       <c r="H24" s="99"/>
-    </row>
-    <row r="25" spans="2:32" ht="350" customHeight="1"/>
-    <row r="26" spans="2:32">
-      <c r="B26" s="107" t="s">
+      <c r="AC24" s="73"/>
+      <c r="AD24" s="73"/>
+      <c r="AE24" s="73"/>
+      <c r="AF24" s="73"/>
+      <c r="AG24" s="73"/>
+    </row>
+    <row r="25" spans="2:33">
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="123"/>
+      <c r="G25" s="123"/>
+      <c r="H25" s="99"/>
+      <c r="AC25" s="128" t="s">
+        <v>508</v>
+      </c>
+      <c r="AD25" s="128">
+        <f>STDEV(AD4:AD22)</f>
+        <v>26.449508599507176</v>
+      </c>
+      <c r="AE25" s="128">
+        <f t="shared" ref="AE25:AG25" si="10">STDEV(AE4:AE22)</f>
+        <v>27.660337593421776</v>
+      </c>
+      <c r="AF25" s="128">
+        <f t="shared" si="10"/>
+        <v>13.547304105814254</v>
+      </c>
+      <c r="AG25" s="128">
+        <f t="shared" si="10"/>
+        <v>9.2392948821241667</v>
+      </c>
+    </row>
+    <row r="26" spans="2:33" ht="350" customHeight="1"/>
+    <row r="27" spans="2:33">
+      <c r="B27" s="109" t="s">
         <v>505</v>
       </c>
-      <c r="C26" s="107"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-    </row>
-    <row r="28" spans="2:32">
-      <c r="B28" s="72" t="s">
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+    </row>
+    <row r="29" spans="2:33">
+      <c r="B29" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="72" t="s">
+      <c r="C29" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="72" t="s">
+      <c r="D29" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E29" s="72" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:32">
-      <c r="B29" s="73">
+    <row r="30" spans="2:33">
+      <c r="B30" s="73">
         <v>1</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C30" s="36">
         <v>68.014414634146334</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D30" s="37">
         <v>1</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E30" s="37">
         <v>6.8</v>
       </c>
     </row>
-    <row r="30" spans="2:32">
-      <c r="B30" s="73">
+    <row r="31" spans="2:33">
+      <c r="B31" s="73">
         <v>2</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C31" s="36">
         <v>100.26741463414632</v>
-      </c>
-      <c r="D30" s="37">
-        <v>5</v>
-      </c>
-      <c r="E30" s="37">
-        <v>18.100000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="2:32">
-      <c r="B31" s="73">
-        <v>3</v>
-      </c>
-      <c r="C31" s="36">
-        <v>132.46873170731703</v>
       </c>
       <c r="D31" s="37">
         <v>5</v>
       </c>
       <c r="E31" s="37">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:33">
+      <c r="B32" s="73">
+        <v>3</v>
+      </c>
+      <c r="C32" s="36">
+        <v>132.46873170731703</v>
+      </c>
+      <c r="D32" s="37">
+        <v>5</v>
+      </c>
+      <c r="E32" s="37">
         <v>12.8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:32">
-      <c r="B32" s="73">
-        <v>4</v>
-      </c>
-      <c r="C32" s="36">
-        <v>154.64156097560979</v>
-      </c>
-      <c r="D32" s="37">
-        <v>7</v>
-      </c>
-      <c r="E32" s="37">
-        <v>15.4</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="73">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" s="36">
-        <v>211.48453658536584</v>
+        <v>154.64156097560979</v>
       </c>
       <c r="D33" s="37">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E33" s="37">
-        <v>14.3</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="73">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" s="36">
-        <v>70.510951219512179</v>
+        <v>211.48453658536584</v>
       </c>
       <c r="D34" s="37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E34" s="37">
-        <v>7.1</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="73">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="36">
-        <v>66.048609756097534</v>
+        <v>70.510951219512179</v>
       </c>
       <c r="D35" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E35" s="37">
-        <v>9.5</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="73">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="36">
-        <v>104.82602439024393</v>
+        <v>66.048609756097534</v>
       </c>
       <c r="D36" s="37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36" s="37">
-        <v>7.4</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="73">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="36">
-        <v>65.420853658536572</v>
+        <v>104.82602439024393</v>
       </c>
       <c r="D37" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" s="37">
-        <v>8.9</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="73">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" s="36">
-        <v>42.585804878048783</v>
+        <v>65.420853658536572</v>
       </c>
       <c r="D38" s="37">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E38" s="37">
-        <v>16.7</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="73">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" s="36">
-        <v>65.473780487804873</v>
+        <v>42.585804878048783</v>
       </c>
       <c r="D39" s="37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E39" s="37">
-        <v>7.4</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="73">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40" s="36">
-        <v>59.81002439024391</v>
+        <v>65.473780487804873</v>
       </c>
       <c r="D40" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40" s="37">
-        <v>14</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="73">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" s="36">
-        <v>37.425292682926823</v>
+        <v>59.81002439024391</v>
       </c>
       <c r="D41" s="37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E41" s="37">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="73">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42" s="36">
-        <v>48.394707317073163</v>
+        <v>37.425292682926823</v>
       </c>
       <c r="D42" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="37">
-        <v>9.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="73">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43" s="36">
-        <v>355.30917073170724</v>
+        <v>48.394707317073163</v>
       </c>
       <c r="D43" s="37">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E43" s="37">
-        <v>29.7</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="73">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44" s="36">
-        <v>20.50239024390244</v>
+        <v>355.30917073170724</v>
       </c>
       <c r="D44" s="37">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E44" s="37">
-        <v>5.6</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="73">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45" s="36">
-        <v>99.988414634146352</v>
+        <v>20.50239024390244</v>
       </c>
       <c r="D45" s="37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E45" s="37">
-        <v>16.2</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="73">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="36">
-        <v>132.07892682926831</v>
+        <v>99.988414634146352</v>
       </c>
       <c r="D46" s="37">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E46" s="37">
-        <v>16.7</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="73">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47" s="36">
-        <v>145.23982926829271</v>
+        <v>132.07892682926831</v>
       </c>
       <c r="D47" s="37">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E47" s="37">
-        <v>21.3</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="73">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48" s="36">
-        <v>80.621829268292686</v>
+        <v>145.23982926829271</v>
       </c>
       <c r="D48" s="37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" s="37">
-        <v>9.8000000000000007</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="73">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49" s="36">
-        <v>89.939219512195123</v>
+        <v>80.621829268292686</v>
       </c>
       <c r="D49" s="37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E49" s="37">
-        <v>11.7</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="73">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C50" s="36">
-        <v>86.29456097560977</v>
+        <v>89.939219512195123</v>
       </c>
       <c r="D50" s="37">
         <v>2</v>
       </c>
       <c r="E50" s="37">
-        <v>10.6</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="73">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="36">
-        <v>54.500707317073157</v>
+        <v>86.29456097560977</v>
       </c>
       <c r="D51" s="37">
         <v>2</v>
       </c>
       <c r="E51" s="37">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" s="73">
+        <v>23</v>
+      </c>
+      <c r="C52" s="36">
+        <v>54.500707317073157</v>
+      </c>
+      <c r="D52" s="37">
+        <v>2</v>
+      </c>
+      <c r="E52" s="37">
         <v>9.6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="C52" s="74" t="s">
-        <v>326</v>
-      </c>
-      <c r="D52" s="74">
-        <f>PEARSON($C29:$C51,D29:D51)</f>
-        <v>0.72591509307923441</v>
-      </c>
-      <c r="E52" s="74">
-        <f>PEARSON($C29:$C51,E29:E51)</f>
-        <v>0.78748899109661075</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="C53" s="74" t="s">
+        <v>326</v>
+      </c>
+      <c r="D53" s="74">
+        <f>PEARSON($C30:$C52,D30:D52)</f>
+        <v>0.72591509307923441</v>
+      </c>
+      <c r="E53" s="74">
+        <f>PEARSON($C30:$C52,E30:E52)</f>
+        <v>0.78748899109661075</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="C54" s="74" t="s">
         <v>327</v>
       </c>
-      <c r="D53" s="38">
+      <c r="D54" s="38">
         <v>0.50800000000000001</v>
       </c>
-      <c r="E53" s="38">
+      <c r="E54" s="38">
         <v>0.48499999999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B26:E26"/>
+  <mergeCells count="6">
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="B27:E27"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="T9:V9"/>
+    <mergeCell ref="X2:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37419,26 +37519,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="121" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="15"/>
@@ -37741,14 +37841,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="3" spans="1:8">
       <c r="F3" s="42">
@@ -38389,13 +38489,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="18"/>
@@ -38715,13 +38815,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="42">
@@ -39037,12 +39137,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
     </row>
     <row r="2" spans="1:6" s="10" customFormat="1"/>
     <row r="3" spans="1:6" s="10" customFormat="1">
@@ -39508,7 +39608,7 @@
   <sheetPr codeName="Feuil64"/>
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:G19"/>
     </sheetView>
   </sheetViews>
@@ -39523,13 +39623,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="19">
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="108" t="s">
         <v>475</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="72" t="s">
@@ -39971,36 +40071,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="19">
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="108" t="s">
         <v>501</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="3" spans="2:8">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="110" t="s">
         <v>471</v>
       </c>
-      <c r="C3" s="109"/>
-      <c r="E3" s="112" t="s">
+      <c r="C3" s="111"/>
+      <c r="E3" s="114" t="s">
         <v>480</v>
       </c>
       <c r="F3" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="G3" s="114" t="s">
+      <c r="G3" s="116" t="s">
         <v>326</v>
       </c>
-      <c r="H3" s="114"/>
+      <c r="H3" s="116"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
-      <c r="E4" s="113"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="113"/>
+      <c r="E4" s="115"/>
       <c r="F4" s="72"/>
       <c r="G4" s="72" t="s">
         <v>503</v>
@@ -40109,14 +40209,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="3" spans="1:11">
       <c r="B3" s="78"/>
@@ -40559,16 +40659,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="29">
@@ -41652,16 +41752,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="22"/>

</xml_diff>

<commit_message>
Adding fMRI Peitek experiment 2021 (#14)
</commit_message>
<xml_diff>
--- a/dataset-cpx.xlsx
+++ b/dataset-cpx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/these/studies/cpx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A5CBF6-416E-F543-9D1E-75E5B083B173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC44FB9-3002-5B46-BE09-2720134F6BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{E3999CCB-9ED0-3445-84E9-42CD1661CA3C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{E3999CCB-9ED0-3445-84E9-42CD1661CA3C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -19,22 +19,22 @@
     <sheet name="siegmund2012" sheetId="27" r:id="rId4"/>
     <sheet name="peitek2021" sheetId="71" r:id="rId5"/>
     <sheet name="Synthesis" sheetId="82" r:id="rId6"/>
-    <sheet name="ArrAvg" sheetId="65" state="hidden" r:id="rId7"/>
-    <sheet name="CountSubstr" sheetId="66" state="hidden" r:id="rId8"/>
-    <sheet name="CountVwls" sheetId="67" state="hidden" r:id="rId9"/>
-    <sheet name="DumbSort" sheetId="68" state="hidden" r:id="rId10"/>
-    <sheet name="GrCoDiv" sheetId="69" state="hidden" r:id="rId11"/>
-    <sheet name="hIndex" sheetId="70" state="hidden" r:id="rId12"/>
-    <sheet name="isHur" sheetId="72" state="hidden" r:id="rId13"/>
-    <sheet name="isPalind" sheetId="73" state="hidden" r:id="rId14"/>
-    <sheet name="lgthLastWd" sheetId="74" state="hidden" r:id="rId15"/>
-    <sheet name="binToDec" sheetId="75" state="hidden" r:id="rId16"/>
-    <sheet name="crosSum" sheetId="76" state="hidden" r:id="rId17"/>
-    <sheet name="n!" sheetId="77" state="hidden" r:id="rId18"/>
-    <sheet name="fibonacci" sheetId="78" state="hidden" r:id="rId19"/>
-    <sheet name="power" sheetId="79" state="hidden" r:id="rId20"/>
-    <sheet name="sqrt" sheetId="80" state="hidden" r:id="rId21"/>
-    <sheet name="yesNo" sheetId="81" state="hidden" r:id="rId22"/>
+    <sheet name="ArrAvg" sheetId="65" r:id="rId7"/>
+    <sheet name="CountSubstr" sheetId="66" r:id="rId8"/>
+    <sheet name="CountVwls" sheetId="67" r:id="rId9"/>
+    <sheet name="DumbSort" sheetId="68" r:id="rId10"/>
+    <sheet name="GrCoDiv" sheetId="69" r:id="rId11"/>
+    <sheet name="hIndex" sheetId="70" r:id="rId12"/>
+    <sheet name="isHur" sheetId="72" r:id="rId13"/>
+    <sheet name="isPalind" sheetId="73" r:id="rId14"/>
+    <sheet name="lgthLastWd" sheetId="74" r:id="rId15"/>
+    <sheet name="binToDec" sheetId="75" r:id="rId16"/>
+    <sheet name="crosSum" sheetId="76" r:id="rId17"/>
+    <sheet name="n!" sheetId="77" r:id="rId18"/>
+    <sheet name="fibonacci" sheetId="78" r:id="rId19"/>
+    <sheet name="power" sheetId="79" r:id="rId20"/>
+    <sheet name="sqrt" sheetId="80" r:id="rId21"/>
+    <sheet name="yesNo" sheetId="81" r:id="rId22"/>
     <sheet name="1" sheetId="3" r:id="rId23"/>
     <sheet name="2" sheetId="4" r:id="rId24"/>
     <sheet name="3" sheetId="23" r:id="rId25"/>
@@ -61,14 +61,6 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Feuil37!$B$7:$C$42</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">siegmund2012!$C$3</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">siegmund2012!$C$4:$C$22</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">siegmund2012!$G$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">siegmund2012!$G$4:$G$22</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">siegmund2012!$C$3</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">siegmund2012!$C$4:$C$22</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">siegmund2012!$G$3</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">siegmund2012!$G$4:$G$22</definedName>
     <definedName name="xdata1" hidden="1">#REF!</definedName>
     <definedName name="xdata2" hidden="1">#REF!</definedName>
     <definedName name="xdata3" hidden="1">#REF!</definedName>
@@ -158,7 +150,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -180,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="513">
   <si>
     <t>snippet_id</t>
   </si>
@@ -6219,7 +6211,19 @@
     <t>dyn2</t>
   </si>
   <si>
-    <t>Linear regression line</t>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Linear regression line / metric</t>
+  </si>
+  <si>
+    <t>Linear regression line / time</t>
+  </si>
+  <si>
+    <t>Forecasted values</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -6396,7 +6400,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6463,8 +6467,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -6590,11 +6600,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6769,6 +6803,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6814,10 +6854,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -10038,7 +10090,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F39DA6A-E70F-004D-A8E4-455A9706DC17}" type="CELLRANGE">
+                    <a:fld id="{716EA338-3C1F-244E-9D51-C4FE0674D0ED}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10071,7 +10123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51348929-3CE8-904D-8782-246BF01051EB}" type="CELLRANGE">
+                    <a:fld id="{A89309CF-6FC5-AC4C-9E2E-FA1C3DF438A5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10104,7 +10156,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{812BA8D4-10F9-2246-8E72-BC438B869F21}" type="CELLRANGE">
+                    <a:fld id="{EEF37AA2-5B25-5D43-AF81-00A49C933ECA}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10137,7 +10189,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0F3FBDB-20E5-CE41-9CD9-9F6DA2B6A509}" type="CELLRANGE">
+                    <a:fld id="{59F77E5C-D7F7-9A43-8BB7-E26CF2C3A096}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10170,7 +10222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FBD59BC-295E-6A45-A49E-7BFDB16F6541}" type="CELLRANGE">
+                    <a:fld id="{FA9E53E0-1275-FB4A-989B-9E716A5E2C44}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10203,7 +10255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7E10F74-FF33-5F4E-A291-CBF4B32EFF9B}" type="CELLRANGE">
+                    <a:fld id="{C717A692-843D-7741-BD7A-FE10C58E523D}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10236,7 +10288,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DE4E1CA-077C-C740-A9D1-D4630E9A6A2B}" type="CELLRANGE">
+                    <a:fld id="{150A85E3-7563-074E-8D9F-B0F19A944249}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10269,7 +10321,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E324EC8-9509-9142-A4DF-178DE429EA5A}" type="CELLRANGE">
+                    <a:fld id="{0640945A-ABFB-7D44-86B1-7F3A6F1EB3C0}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10302,7 +10354,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A1387D7-EFB1-054E-AACF-929E55FC7FBD}" type="CELLRANGE">
+                    <a:fld id="{3698AF80-6535-D24A-9597-D52D38946EA7}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10335,7 +10387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{847C2912-4AE9-2B4A-8612-651823491E89}" type="CELLRANGE">
+                    <a:fld id="{79E07AE9-D24A-F141-9DDB-B509FF55543A}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10368,7 +10420,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1824833-361C-0043-950A-3A2A1D29199D}" type="CELLRANGE">
+                    <a:fld id="{30E752C9-4F93-C448-ADB4-0A4B7EA88890}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10401,7 +10453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6A36DEE-156F-3C46-8796-44474D28D323}" type="CELLRANGE">
+                    <a:fld id="{D00D42D9-51F8-7E43-9329-29A38E2C0414}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10434,7 +10486,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6279345F-23FB-EC4F-AB0B-E32FA94A3D88}" type="CELLRANGE">
+                    <a:fld id="{D0A7A321-56F6-8D4F-87CA-A8FF48CF9074}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10467,7 +10519,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3084130C-DCF6-F246-B0CC-B0BE97F0A1C5}" type="CELLRANGE">
+                    <a:fld id="{1737EA59-78B8-2F4E-906F-B6BE8A95EFF5}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10500,7 +10552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1842C9B-B8B9-3747-A93C-1FD3834DDB66}" type="CELLRANGE">
+                    <a:fld id="{B6F109F0-25FF-4145-88D1-AC600ABC5512}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10533,7 +10585,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DD2E44E-D086-E042-9596-A11826EB5F63}" type="CELLRANGE">
+                    <a:fld id="{BAA2942A-5DF6-7840-B8F4-9599242F271C}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10566,7 +10618,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99165BB0-3594-4840-828C-49DA02FD464F}" type="CELLRANGE">
+                    <a:fld id="{DBC37C18-EC5A-224D-953D-7211BDCC346F}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10599,7 +10651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C697E4E9-7030-E847-9A41-B68DA8656610}" type="CELLRANGE">
+                    <a:fld id="{EBA822DF-BAC8-B54B-9A5D-5D219C0C5448}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10632,7 +10684,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44DCBF68-1548-F04E-B0E7-EB1A600AFDC0}" type="CELLRANGE">
+                    <a:fld id="{4FED90A4-D7A3-AD45-B36C-BA066BFDA48E}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10665,7 +10717,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A0650A8-834E-2543-AA9A-8673BB3F5FC1}" type="CELLRANGE">
+                    <a:fld id="{271AA26E-BD2A-CB4D-8D79-AE1F2BFB55E9}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10698,7 +10750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93F49A16-9BFA-6547-B498-DA637D6C51CB}" type="CELLRANGE">
+                    <a:fld id="{62E5FAF4-5638-454A-9361-30DD38464D45}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10731,7 +10783,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9385C19-D00E-5C46-A844-228595570F8C}" type="CELLRANGE">
+                    <a:fld id="{0C0A1082-9DCA-6E42-A349-405022DC45BA}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -10764,7 +10816,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54E06FA0-E2D3-5C4D-AEBD-0F6C3D52159E}" type="CELLRANGE">
+                    <a:fld id="{2E494FA3-0F9C-FE4F-8159-A77B639F5CBD}" type="CELLRANGE">
                       <a:rPr lang="fr-FR"/>
                       <a:pPr/>
                       <a:t>[PLAGECELL]</a:t>
@@ -11742,7 +11794,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>siegmund2012!$E$28</c:f>
+              <c:f>siegmund2012!$E$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11804,7 +11856,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>siegmund2012!$C$29:$C$51</c:f>
+              <c:f>siegmund2012!$C$30:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="23"/>
@@ -11882,7 +11934,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>siegmund2012!$E$29:$E$51</c:f>
+              <c:f>siegmund2012!$E$30:$E$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -13544,7 +13596,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>siegmund2012!$D$28</c:f>
+              <c:f>siegmund2012!$D$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13591,7 +13643,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>siegmund2012!$C$29:$C$51</c:f>
+              <c:f>siegmund2012!$C$30:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="23"/>
@@ -13669,7 +13721,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>siegmund2012!$D$29:$D$51</c:f>
+              <c:f>siegmund2012!$D$30:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
@@ -22274,13 +22326,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>336313</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>11759</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>740832</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>47037</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22316,8 +22368,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>776111</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>11760</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>188148</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22346,13 +22398,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>399815</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>30339</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>799630</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>3974630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22382,13 +22434,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>154046</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>33631</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>364537</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>3998148</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22418,13 +22470,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>142287</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>10112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>281046</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>23518</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22454,13 +22506,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>89370</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>492242</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>545630</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>4127499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -22489,15 +22541,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>492242</xdr:rowOff>
+      <xdr:colOff>606778</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>504001</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>204612</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>4139259</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>239889</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>4151018</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23592,16 +23644,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="2" spans="1:25">
       <c r="B2" s="14"/>
@@ -25092,16 +25144,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
     </row>
     <row r="3" spans="1:10">
       <c r="H3" s="29">
@@ -25607,14 +25659,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
     </row>
     <row r="3" spans="1:8">
       <c r="F3" s="26">
@@ -25977,15 +26029,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
     </row>
     <row r="3" spans="1:9">
       <c r="D3" s="31"/>
@@ -26469,12 +26521,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
     </row>
     <row r="3" spans="1:6">
       <c r="D3" s="26">
@@ -26646,15 +26698,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
     </row>
     <row r="3" spans="1:8">
       <c r="B3" s="76"/>
@@ -26922,15 +26974,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="26">
@@ -27763,13 +27815,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="29">
@@ -28030,13 +28082,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="3" spans="1:7">
       <c r="D3" s="76"/>
@@ -28329,12 +28381,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
     </row>
     <row r="3" spans="1:6">
       <c r="D3" s="29">
@@ -28564,12 +28616,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
     </row>
     <row r="3" spans="1:6">
       <c r="D3" s="29">
@@ -29150,13 +29202,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="29">
@@ -29429,13 +29481,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="29">
@@ -29980,10 +30032,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="117"/>
+      <c r="B1" s="119"/>
     </row>
     <row r="3" spans="1:5">
       <c r="C3" s="26">
@@ -30139,7 +30191,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScale="137" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30149,12 +30201,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
     </row>
     <row r="2" spans="1:7" ht="19">
       <c r="A2" s="20"/>
@@ -30446,14 +30498,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="3" spans="1:8">
       <c r="G3" s="42">
@@ -30994,14 +31046,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="2" spans="1:9" ht="19">
       <c r="A2" s="53"/>
@@ -31614,14 +31666,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="42">
@@ -32118,13 +32170,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:6" s="10" customFormat="1">
       <c r="A2" s="57"/>
@@ -32411,13 +32463,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:7" s="10" customFormat="1"/>
     <row r="3" spans="1:7" s="10" customFormat="1">
@@ -33402,13 +33454,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="75"/>
@@ -33688,14 +33740,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1"/>
     <row r="3" spans="1:8" s="10" customFormat="1">
@@ -34205,13 +34257,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="41">
@@ -34390,14 +34442,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1">
       <c r="A2" s="11"/>
@@ -34618,14 +34670,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1">
       <c r="A2" s="13"/>
@@ -34840,13 +34892,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="13"/>
@@ -35024,13 +35076,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="42">
@@ -35378,13 +35430,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="42">
@@ -35507,15 +35559,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="42">
@@ -35737,10 +35789,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B752191-782E-EA48-B322-664FAB9CF9B3}">
   <sheetPr codeName="Feuil3"/>
-  <dimension ref="B1:AH53"/>
+  <dimension ref="B1:AG54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView topLeftCell="M1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2:AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -35755,27 +35807,41 @@
     <col min="8" max="8" width="10.5" style="1" customWidth="1"/>
     <col min="9" max="18" width="10.83203125" style="1"/>
     <col min="19" max="19" width="4.1640625" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="1"/>
+    <col min="20" max="27" width="10.83203125" style="1"/>
+    <col min="28" max="28" width="3.6640625" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="19">
-      <c r="B1" s="106" t="s">
+    <row r="1" spans="2:33" ht="19">
+      <c r="B1" s="108" t="s">
         <v>474</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-    </row>
-    <row r="2" spans="2:34">
-      <c r="T2" s="121" t="s">
-        <v>508</v>
-      </c>
-      <c r="U2" s="121"/>
-      <c r="V2" s="121"/>
-    </row>
-    <row r="3" spans="2:34">
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+    </row>
+    <row r="2" spans="2:33">
+      <c r="T2" s="116" t="s">
+        <v>509</v>
+      </c>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="X2" s="124" t="s">
+        <v>511</v>
+      </c>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="126"/>
+      <c r="AD2" s="116" t="s">
+        <v>512</v>
+      </c>
+      <c r="AE2" s="116"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="116"/>
+    </row>
+    <row r="3" spans="2:33">
       <c r="B3" s="72" t="s">
         <v>502</v>
       </c>
@@ -35797,55 +35863,52 @@
         <v>dyn2</v>
       </c>
       <c r="H3" s="99"/>
-      <c r="T3" s="1" t="str">
+      <c r="T3" s="73" t="str">
         <f>D3</f>
         <v>sonarqube</v>
       </c>
-      <c r="U3" s="1" cm="1">
+      <c r="U3" s="73" cm="1">
         <f t="array" ref="U3:V3">LINEST(D4:D22,C4:C22)</f>
         <v>2.4558162269338261E-2</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="73">
         <v>0.68727428091925669</v>
       </c>
-      <c r="X3" s="14" t="str">
+      <c r="X3" s="106" t="str">
         <f>D3</f>
         <v>sonarqube</v>
       </c>
-      <c r="Y3" s="14" t="str">
+      <c r="Y3" s="106" t="str">
         <f>E3</f>
         <v>genese_cpx</v>
       </c>
-      <c r="Z3" s="14" t="str">
+      <c r="Z3" s="106" t="str">
         <f>F3</f>
         <v>dyn1</v>
       </c>
-      <c r="AA3" s="14" t="str">
+      <c r="AA3" s="106" t="str">
         <f>G3</f>
         <v>dyn2</v>
       </c>
-      <c r="AC3" s="14" t="str">
+      <c r="AB3" s="107"/>
+      <c r="AD3" s="106" t="str">
         <f>D3</f>
         <v>sonarqube</v>
       </c>
-      <c r="AD3" s="14" t="str">
+      <c r="AE3" s="106" t="str">
         <f>E3</f>
         <v>genese_cpx</v>
       </c>
-      <c r="AE3" s="14" t="str">
+      <c r="AF3" s="106" t="str">
         <f>F3</f>
         <v>dyn1</v>
       </c>
-      <c r="AF3" s="14" t="str">
+      <c r="AG3" s="106" t="str">
         <f>G3</f>
         <v>dyn2</v>
       </c>
-      <c r="AH3" s="1">
-        <f>STDEV(X4:X22)</f>
-        <v>25.675427112967437</v>
-      </c>
-    </row>
-    <row r="4" spans="2:34">
+    </row>
+    <row r="4" spans="2:33">
       <c r="B4" s="37">
         <v>1</v>
       </c>
@@ -35867,51 +35930,51 @@
         <v>4.8948</v>
       </c>
       <c r="H4" s="99"/>
-      <c r="T4" s="1" t="str">
+      <c r="T4" s="73" t="str">
         <f>E3</f>
         <v>genese_cpx</v>
       </c>
-      <c r="U4" s="1" cm="1">
+      <c r="U4" s="73" cm="1">
         <f t="array" ref="U4:V4">LINEST(E4:E22,C4:C22)</f>
         <v>5.5463678990432835E-2</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="73">
         <v>6.7027076730524611</v>
       </c>
-      <c r="X4" s="1">
-        <f>$D4*$U$10+$V$10</f>
+      <c r="X4" s="73">
+        <f t="shared" ref="X4:X22" si="0">$D4*$U$10+$V$10</f>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y4" s="1">
-        <f>E4*$U$11+$V$11</f>
+      <c r="Y4" s="73">
+        <f t="shared" ref="Y4:Y22" si="1">E4*$U$11+$V$11</f>
         <v>58.202273239029132</v>
       </c>
-      <c r="Z4" s="1">
-        <f>F4*$U$12+$V$12</f>
+      <c r="Z4" s="73">
+        <f t="shared" ref="Z4:Z22" si="2">F4*$U$12+$V$12</f>
         <v>51.752996067965306</v>
       </c>
-      <c r="AA4" s="1">
-        <f>G4*$U$13+$V$13</f>
+      <c r="AA4" s="73">
+        <f t="shared" ref="AA4:AA22" si="3">G4*$U$13+$V$13</f>
         <v>58.230202971233552</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AD4" s="73">
         <f>ABS($C4-X4)</f>
         <v>6.5974958013937197</v>
       </c>
-      <c r="AD4" s="1">
-        <f t="shared" ref="AD4:AF19" si="0">ABS($C4-Y4)</f>
+      <c r="AE4" s="73">
+        <f>ABS($C4-Y4)</f>
         <v>9.8121413951172016</v>
       </c>
-      <c r="AE4" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF4" s="73">
+        <f>ABS($C4-Z4)</f>
         <v>16.261418566181028</v>
       </c>
-      <c r="AF4" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG4" s="73">
+        <f>ABS($C4-AA4)</f>
         <v>9.7842116629127815</v>
       </c>
     </row>
-    <row r="5" spans="2:34">
+    <row r="5" spans="2:33">
       <c r="B5" s="37">
         <v>2</v>
       </c>
@@ -35933,51 +35996,51 @@
         <v>7.7837939390651911</v>
       </c>
       <c r="H5" s="99"/>
-      <c r="T5" s="1" t="str">
+      <c r="T5" s="73" t="str">
         <f>F3</f>
         <v>dyn1</v>
       </c>
-      <c r="U5" s="1" cm="1">
+      <c r="U5" s="73" cm="1">
         <f t="array" ref="U5:V5">LINEST(F4:F22,C4:C22)</f>
         <v>7.6128649226312323E-2</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="73">
         <v>1.4159069751836109</v>
       </c>
-      <c r="X5" s="1">
-        <f>$D5*$U$10+$V$10</f>
+      <c r="X5" s="73">
+        <f t="shared" si="0"/>
         <v>112.1775137456446</v>
       </c>
-      <c r="Y5" s="1">
-        <f>E5*$U$11+$V$11</f>
+      <c r="Y5" s="73">
+        <f t="shared" si="1"/>
         <v>121.17951911274326</v>
       </c>
-      <c r="Z5" s="1">
-        <f>F5*$U$12+$V$12</f>
+      <c r="Z5" s="73">
+        <f t="shared" si="2"/>
         <v>113.07798598541521</v>
       </c>
-      <c r="AA5" s="1">
-        <f>G5*$U$13+$V$13</f>
+      <c r="AA5" s="73">
+        <f t="shared" si="3"/>
         <v>114.54182119618963</v>
       </c>
-      <c r="AC5" s="1">
-        <f t="shared" ref="AC5:AC22" si="1">ABS($C5-X5)</f>
+      <c r="AD5" s="73">
+        <f t="shared" ref="AD5:AD22" si="4">ABS($C5-X5)</f>
         <v>11.910099111498283</v>
       </c>
-      <c r="AD5" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE5" s="73">
+        <f>ABS($C5-Y5)</f>
         <v>20.912104478596945</v>
       </c>
-      <c r="AE5" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF5" s="73">
+        <f>ABS($C5-Z5)</f>
         <v>12.810571351268891</v>
       </c>
-      <c r="AF5" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG5" s="73">
+        <f>ABS($C5-AA5)</f>
         <v>14.27440656204331</v>
       </c>
     </row>
-    <row r="6" spans="2:34">
+    <row r="6" spans="2:33">
       <c r="B6" s="37">
         <v>4</v>
       </c>
@@ -35999,51 +36062,51 @@
         <v>9.3121798400000007</v>
       </c>
       <c r="H6" s="99"/>
-      <c r="T6" s="1" t="str">
+      <c r="T6" s="73" t="str">
         <f>G3</f>
         <v>dyn2</v>
       </c>
-      <c r="U6" s="1" cm="1">
+      <c r="U6" s="73" cm="1">
         <f t="array" ref="U6:V6">LINEST(G4:G22,C4:C22)</f>
         <v>4.4544978836098509E-2</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="73">
         <v>2.4714422904012738</v>
       </c>
-      <c r="X6" s="1">
-        <f>$D6*$U$10+$V$10</f>
+      <c r="X6" s="73">
+        <f t="shared" si="0"/>
         <v>137.55781120209062</v>
       </c>
-      <c r="Y6" s="1">
-        <f>E6*$U$11+$V$11</f>
+      <c r="Y6" s="73">
+        <f t="shared" si="1"/>
         <v>106.13185859424519</v>
       </c>
-      <c r="Z6" s="1">
-        <f>F6*$U$12+$V$12</f>
+      <c r="Z6" s="73">
+        <f t="shared" si="2"/>
         <v>162.09344766569455</v>
       </c>
-      <c r="AA6" s="1">
-        <f>G6*$U$13+$V$13</f>
+      <c r="AA6" s="73">
+        <f t="shared" si="3"/>
         <v>144.33277443775143</v>
       </c>
-      <c r="AC6" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD6" s="73">
+        <f t="shared" si="4"/>
         <v>17.083749773519173</v>
       </c>
-      <c r="AD6" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE6" s="73">
+        <f>ABS($C6-Y6)</f>
         <v>48.509702381364605</v>
       </c>
-      <c r="AE6" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF6" s="73">
+        <f>ABS($C6-Z6)</f>
         <v>7.4518866900847627</v>
       </c>
-      <c r="AF6" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG6" s="73">
+        <f>ABS($C6-AA6)</f>
         <v>10.308786537858367</v>
       </c>
     </row>
-    <row r="7" spans="2:34">
+    <row r="7" spans="2:33">
       <c r="B7" s="37">
         <v>5</v>
       </c>
@@ -36065,40 +36128,40 @@
         <v>11.704923999999998</v>
       </c>
       <c r="H7" s="99"/>
-      <c r="X7" s="1">
-        <f>$D7*$U$10+$V$10</f>
+      <c r="X7" s="73">
+        <f t="shared" si="0"/>
         <v>112.1775137456446</v>
       </c>
-      <c r="Y7" s="1">
-        <f>E7*$U$11+$V$11</f>
+      <c r="Y7" s="73">
+        <f t="shared" si="1"/>
         <v>100.00133023485711</v>
       </c>
-      <c r="Z7" s="1">
-        <f>F7*$U$12+$V$12</f>
+      <c r="Z7" s="73">
+        <f t="shared" si="2"/>
         <v>189.67856056512687</v>
       </c>
-      <c r="AA7" s="1">
-        <f>G7*$U$13+$V$13</f>
+      <c r="AA7" s="73">
+        <f t="shared" si="3"/>
         <v>190.97160390220904</v>
       </c>
-      <c r="AC7" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD7" s="73">
+        <f t="shared" si="4"/>
         <v>99.307022839721242</v>
       </c>
-      <c r="AD7" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE7" s="73">
+        <f>ABS($C7-Y7)</f>
         <v>111.48320635050874</v>
       </c>
-      <c r="AE7" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF7" s="73">
+        <f>ABS($C7-Z7)</f>
         <v>21.805976020238973</v>
       </c>
-      <c r="AF7" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG7" s="73">
+        <f>ABS($C7-AA7)</f>
         <v>20.512932683156805</v>
       </c>
     </row>
-    <row r="8" spans="2:34">
+    <row r="8" spans="2:33">
       <c r="B8" s="37">
         <v>6</v>
       </c>
@@ -36120,40 +36183,40 @@
         <v>4.7900520000000002</v>
       </c>
       <c r="H8" s="99"/>
-      <c r="X8" s="1">
-        <f>$D8*$U$10+$V$10</f>
+      <c r="X8" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y8" s="1">
-        <f>E8*$U$11+$V$11</f>
+      <c r="Y8" s="73">
+        <f t="shared" si="1"/>
         <v>59.87423551886225</v>
       </c>
-      <c r="Z8" s="1">
-        <f>F8*$U$12+$V$12</f>
+      <c r="Z8" s="73">
+        <f t="shared" si="2"/>
         <v>53.723361275067617</v>
       </c>
-      <c r="AA8" s="1">
-        <f>G8*$U$13+$V$13</f>
+      <c r="AA8" s="73">
+        <f t="shared" si="3"/>
         <v>56.18847858196871</v>
       </c>
-      <c r="AC8" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD8" s="73">
+        <f t="shared" si="4"/>
         <v>9.0940323867595652</v>
       </c>
-      <c r="AD8" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE8" s="73">
+        <f>ABS($C8-Y8)</f>
         <v>10.63671570064993</v>
       </c>
-      <c r="AE8" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF8" s="73">
+        <f>ABS($C8-Z8)</f>
         <v>16.787589944444562</v>
       </c>
-      <c r="AF8" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG8" s="73">
+        <f>ABS($C8-AA8)</f>
         <v>14.32247263754347</v>
       </c>
     </row>
-    <row r="9" spans="2:34">
+    <row r="9" spans="2:33">
       <c r="B9" s="37">
         <v>7</v>
       </c>
@@ -36175,45 +36238,45 @@
         <v>6.6073685280000003</v>
       </c>
       <c r="H9" s="99"/>
-      <c r="T9" s="121" t="s">
-        <v>508</v>
-      </c>
-      <c r="U9" s="121"/>
-      <c r="V9" s="121"/>
-      <c r="X9" s="1">
-        <f>$D9*$U$10+$V$10</f>
+      <c r="T9" s="116" t="s">
+        <v>510</v>
+      </c>
+      <c r="U9" s="116"/>
+      <c r="V9" s="116"/>
+      <c r="X9" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y9" s="1">
-        <f>E9*$U$11+$V$11</f>
+      <c r="Y9" s="73">
+        <f t="shared" si="1"/>
         <v>73.249933757527202</v>
       </c>
-      <c r="Z9" s="1">
-        <f>F9*$U$12+$V$12</f>
+      <c r="Z9" s="73">
+        <f t="shared" si="2"/>
         <v>98.54916973664514</v>
       </c>
-      <c r="AA9" s="1">
-        <f>G9*$U$13+$V$13</f>
+      <c r="AA9" s="73">
+        <f t="shared" si="3"/>
         <v>91.611202435710055</v>
       </c>
-      <c r="AC9" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD9" s="73">
+        <f t="shared" si="4"/>
         <v>20.748606533101082</v>
       </c>
-      <c r="AD9" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE9" s="73">
+        <f>ABS($C9-Y9)</f>
         <v>7.2013240014296684</v>
       </c>
-      <c r="AE9" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF9" s="73">
+        <f>ABS($C9-Z9)</f>
         <v>32.500559980547607</v>
       </c>
-      <c r="AF9" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG9" s="73">
+        <f>ABS($C9-AA9)</f>
         <v>25.562592679612521</v>
       </c>
     </row>
-    <row r="10" spans="2:34">
+    <row r="10" spans="2:33">
       <c r="B10" s="103">
         <v>8</v>
       </c>
@@ -36235,51 +36298,51 @@
         <v>6.8864000000000001</v>
       </c>
       <c r="H10" s="99"/>
-      <c r="T10" s="1" t="str">
+      <c r="T10" s="73" t="str">
         <f>T3</f>
         <v>sonarqube</v>
       </c>
-      <c r="U10" s="1" cm="1">
+      <c r="U10" s="73" cm="1">
         <f t="array" ref="U10:V10">LINEST(C4:C22,D4:D22)</f>
         <v>12.690148728222999</v>
       </c>
-      <c r="V10" s="1">
+      <c r="V10" s="73">
         <v>48.726770104529614</v>
       </c>
-      <c r="X10" s="1">
-        <f>$D10*$U$10+$V$10</f>
+      <c r="X10" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y10" s="1">
-        <f>E10*$U$11+$V$11</f>
+      <c r="Y10" s="73">
+        <f t="shared" si="1"/>
         <v>61.546197798695374</v>
       </c>
-      <c r="Z10" s="1">
-        <f>F10*$U$12+$V$12</f>
+      <c r="Z10" s="73">
+        <f t="shared" si="2"/>
         <v>90.175117606460319</v>
       </c>
-      <c r="AA10" s="1">
-        <f>G10*$U$13+$V$13</f>
+      <c r="AA10" s="73">
+        <f t="shared" si="3"/>
         <v>97.050020950191168</v>
       </c>
-      <c r="AC10" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD10" s="73">
+        <f t="shared" si="4"/>
         <v>43.409105557491316</v>
       </c>
-      <c r="AD10" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE10" s="73">
+        <f>ABS($C10-Y10)</f>
         <v>43.279826591548556</v>
       </c>
-      <c r="AE10" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF10" s="73">
+        <f>ABS($C10-Z10)</f>
         <v>14.650906783783611</v>
       </c>
-      <c r="AF10" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG10" s="73">
+        <f>ABS($C10-AA10)</f>
         <v>7.7760034400527616</v>
       </c>
     </row>
-    <row r="11" spans="2:34">
+    <row r="11" spans="2:33">
       <c r="B11" s="103">
         <v>9</v>
       </c>
@@ -36301,51 +36364,51 @@
         <v>5.1806567180919743</v>
       </c>
       <c r="H11" s="99"/>
-      <c r="T11" s="1" t="str">
-        <f t="shared" ref="T11:T13" si="2">T4</f>
+      <c r="T11" s="73" t="str">
+        <f t="shared" ref="T11:T13" si="5">T4</f>
         <v>genese_cpx</v>
       </c>
-      <c r="U11" s="1" cm="1">
+      <c r="U11" s="73" cm="1">
         <f t="array" ref="U11:V11">LINEST(C4:C22,E4:E22)</f>
         <v>5.5732075994437276</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V11" s="73">
         <v>20.304461562811788</v>
       </c>
-      <c r="X11" s="1">
-        <f>$D11*$U$10+$V$10</f>
+      <c r="X11" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y11" s="1">
-        <f>E11*$U$11+$V$11</f>
+      <c r="Y11" s="73">
+        <f t="shared" si="1"/>
         <v>69.906009197860968</v>
       </c>
-      <c r="Z11" s="1">
-        <f>F11*$U$12+$V$12</f>
+      <c r="Z11" s="73">
+        <f t="shared" si="2"/>
         <v>78.96262041061054</v>
       </c>
-      <c r="AA11" s="1">
-        <f>G11*$U$13+$V$13</f>
+      <c r="AA11" s="73">
+        <f t="shared" si="3"/>
         <v>63.802057643051512</v>
       </c>
-      <c r="AC11" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD11" s="73">
+        <f t="shared" si="4"/>
         <v>21.376362630662044</v>
       </c>
-      <c r="AD11" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE11" s="73">
+        <f>ABS($C11-Y11)</f>
         <v>4.4851555393243956</v>
       </c>
-      <c r="AE11" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF11" s="73">
+        <f>ABS($C11-Z11)</f>
         <v>13.541766752073968</v>
       </c>
-      <c r="AF11" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG11" s="73">
+        <f>ABS($C11-AA11)</f>
         <v>1.61879601548506</v>
       </c>
     </row>
-    <row r="12" spans="2:34">
+    <row r="12" spans="2:33">
       <c r="B12" s="103">
         <v>10</v>
       </c>
@@ -36367,51 +36430,51 @@
         <v>6.0659999999999989</v>
       </c>
       <c r="H12" s="99"/>
-      <c r="T12" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="T12" s="73" t="str">
+        <f t="shared" si="5"/>
         <v>dyn1</v>
       </c>
-      <c r="U12" s="1" cm="1">
+      <c r="U12" s="73" cm="1">
         <f t="array" ref="U12:V12">LINEST(C4:C22,F4:F22)</f>
         <v>10.262318786991187</v>
       </c>
-      <c r="V12" s="1">
+      <c r="V12" s="73">
         <v>3.7253441448465452</v>
       </c>
-      <c r="X12" s="1">
-        <f>$D12*$U$10+$V$10</f>
+      <c r="X12" s="73">
+        <f t="shared" si="0"/>
         <v>124.8676624738676</v>
       </c>
-      <c r="Y12" s="1">
-        <f>E12*$U$11+$V$11</f>
+      <c r="Y12" s="73">
+        <f t="shared" si="1"/>
         <v>113.37702847352205</v>
       </c>
-      <c r="Z12" s="1">
-        <f>F12*$U$12+$V$12</f>
+      <c r="Z12" s="73">
+        <f t="shared" si="2"/>
         <v>96.086213227767232</v>
       </c>
-      <c r="AA12" s="1">
-        <f>G12*$U$13+$V$13</f>
+      <c r="AA12" s="73">
+        <f t="shared" si="3"/>
         <v>81.058969197862965</v>
       </c>
-      <c r="AC12" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD12" s="73">
+        <f t="shared" si="4"/>
         <v>82.281857595818821</v>
       </c>
-      <c r="AD12" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE12" s="73">
+        <f>ABS($C12-Y12)</f>
         <v>70.791223595473269</v>
       </c>
-      <c r="AE12" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF12" s="73">
+        <f>ABS($C12-Z12)</f>
         <v>53.500408349718448</v>
       </c>
-      <c r="AF12" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG12" s="73">
+        <f>ABS($C12-AA12)</f>
         <v>38.473164319814181</v>
       </c>
     </row>
-    <row r="13" spans="2:34">
+    <row r="13" spans="2:33">
       <c r="B13" s="103">
         <v>11</v>
       </c>
@@ -36433,51 +36496,51 @@
         <v>4.976</v>
       </c>
       <c r="H13" s="99"/>
-      <c r="T13" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="T13" s="73" t="str">
+        <f t="shared" si="5"/>
         <v>dyn2</v>
       </c>
-      <c r="U13" s="1" cm="1">
+      <c r="U13" s="73" cm="1">
         <f t="array" ref="U13:V13">LINEST(C4:C22,G4:G22)</f>
         <v>19.491774442135785</v>
       </c>
-      <c r="V13" s="1">
+      <c r="V13" s="73">
         <v>-37.178134568132691</v>
       </c>
-      <c r="X13" s="1">
-        <f>$D13*$U$10+$V$10</f>
+      <c r="X13" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y13" s="1">
-        <f>E13*$U$11+$V$11</f>
+      <c r="Y13" s="73">
+        <f t="shared" si="1"/>
         <v>61.546197798695374</v>
       </c>
-      <c r="Z13" s="1">
-        <f>F13*$U$12+$V$12</f>
+      <c r="Z13" s="73">
+        <f t="shared" si="2"/>
         <v>71.456648138988385</v>
       </c>
-      <c r="AA13" s="1">
-        <f>G13*$U$13+$V$13</f>
+      <c r="AA13" s="73">
+        <f t="shared" si="3"/>
         <v>59.812935055934972</v>
       </c>
-      <c r="AC13" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD13" s="73">
+        <f t="shared" si="4"/>
         <v>4.0568616550522592</v>
       </c>
-      <c r="AD13" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE13" s="73">
+        <f>ABS($C13-Y13)</f>
         <v>3.9275826891094994</v>
       </c>
-      <c r="AE13" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF13" s="73">
+        <f>ABS($C13-Z13)</f>
         <v>5.9828676511835113</v>
       </c>
-      <c r="AF13" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG13" s="73">
+        <f>ABS($C13-AA13)</f>
         <v>5.6608454318699017</v>
       </c>
     </row>
-    <row r="14" spans="2:34">
+    <row r="14" spans="2:33">
       <c r="B14" s="103">
         <v>12</v>
       </c>
@@ -36499,40 +36562,40 @@
         <v>4.8332000000000006</v>
       </c>
       <c r="H14" s="99"/>
-      <c r="X14" s="1">
-        <f>$D14*$U$10+$V$10</f>
+      <c r="X14" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y14" s="1">
-        <f>E14*$U$11+$V$11</f>
+      <c r="Y14" s="73">
+        <f t="shared" si="1"/>
         <v>98.329367955023969</v>
       </c>
-      <c r="Z14" s="1">
-        <f>F14*$U$12+$V$12</f>
+      <c r="Z14" s="73">
+        <f t="shared" si="2"/>
         <v>61.194329351997197</v>
       </c>
-      <c r="AA14" s="1">
-        <f>G14*$U$13+$V$13</f>
+      <c r="AA14" s="73">
+        <f t="shared" si="3"/>
         <v>57.029509665597999</v>
       </c>
-      <c r="AC14" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD14" s="73">
+        <f t="shared" si="4"/>
         <v>26.987191898954705</v>
       </c>
-      <c r="AD14" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE14" s="73">
+        <f>ABS($C14-Y14)</f>
         <v>38.519343564780058</v>
       </c>
-      <c r="AE14" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF14" s="73">
+        <f>ABS($C14-Z14)</f>
         <v>1.384304961753287</v>
       </c>
-      <c r="AF14" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG14" s="73">
+        <f>ABS($C14-AA14)</f>
         <v>2.7805147246459114</v>
       </c>
     </row>
-    <row r="15" spans="2:34">
+    <row r="15" spans="2:33">
       <c r="B15" s="103">
         <v>13</v>
       </c>
@@ -36554,40 +36617,40 @@
         <v>3</v>
       </c>
       <c r="H15" s="99"/>
-      <c r="X15" s="1">
-        <f>$D15*$U$10+$V$10</f>
+      <c r="X15" s="73">
+        <f t="shared" si="0"/>
         <v>48.726770104529614</v>
       </c>
-      <c r="Y15" s="1">
-        <f>E15*$U$11+$V$11</f>
+      <c r="Y15" s="73">
+        <f t="shared" si="1"/>
         <v>53.743707159474155</v>
       </c>
-      <c r="Z15" s="1">
-        <f>F15*$U$12+$V$12</f>
+      <c r="Z15" s="73">
+        <f t="shared" si="2"/>
         <v>34.512300505820107</v>
       </c>
-      <c r="AA15" s="1">
-        <f>G15*$U$13+$V$13</f>
+      <c r="AA15" s="73">
+        <f t="shared" si="3"/>
         <v>21.297188758274665</v>
       </c>
-      <c r="AC15" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD15" s="73">
+        <f t="shared" si="4"/>
         <v>11.30147742160279</v>
       </c>
-      <c r="AD15" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE15" s="73">
+        <f>ABS($C15-Y15)</f>
         <v>16.318414476547332</v>
       </c>
-      <c r="AE15" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF15" s="73">
+        <f>ABS($C15-Z15)</f>
         <v>2.912992177106716</v>
       </c>
-      <c r="AF15" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG15" s="73">
+        <f>ABS($C15-AA15)</f>
         <v>16.128103924652159</v>
       </c>
     </row>
-    <row r="16" spans="2:34">
+    <row r="16" spans="2:33">
       <c r="B16" s="103">
         <v>14</v>
       </c>
@@ -36609,40 +36672,40 @@
         <v>5.4130162525952006</v>
       </c>
       <c r="H16" s="99"/>
-      <c r="X16" s="1">
-        <f>$D16*$U$10+$V$10</f>
+      <c r="X16" s="73">
+        <f t="shared" si="0"/>
         <v>61.416918832752614</v>
       </c>
-      <c r="Y16" s="1">
-        <f>E16*$U$11+$V$11</f>
+      <c r="Y16" s="73">
+        <f t="shared" si="1"/>
         <v>73.249933757527202</v>
       </c>
-      <c r="Z16" s="1">
-        <f>F16*$U$12+$V$12</f>
+      <c r="Z16" s="73">
+        <f t="shared" si="2"/>
         <v>54.511507357908535</v>
       </c>
-      <c r="AA16" s="1">
-        <f>G16*$U$13+$V$13</f>
+      <c r="AA16" s="73">
+        <f t="shared" si="3"/>
         <v>68.331157279068066</v>
       </c>
-      <c r="AC16" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD16" s="73">
+        <f t="shared" si="4"/>
         <v>13.022211515679452</v>
       </c>
-      <c r="AD16" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE16" s="73">
+        <f>ABS($C16-Y16)</f>
         <v>24.85522644045404</v>
       </c>
-      <c r="AE16" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF16" s="73">
+        <f>ABS($C16-Z16)</f>
         <v>6.116800040835372</v>
       </c>
-      <c r="AF16" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG16" s="73">
+        <f>ABS($C16-AA16)</f>
         <v>19.936449961994903</v>
       </c>
     </row>
-    <row r="17" spans="2:32">
+    <row r="17" spans="2:33">
       <c r="B17" s="103">
         <v>16</v>
       </c>
@@ -36664,40 +36727,40 @@
         <v>2</v>
       </c>
       <c r="H17" s="99"/>
-      <c r="X17" s="1">
-        <f>$D17*$U$10+$V$10</f>
+      <c r="X17" s="73">
+        <f t="shared" si="0"/>
         <v>48.726770104529614</v>
       </c>
-      <c r="Y17" s="1">
-        <f>E17*$U$11+$V$11</f>
+      <c r="Y17" s="73">
+        <f t="shared" si="1"/>
         <v>51.514424119696656</v>
       </c>
-      <c r="Z17" s="1">
-        <f>F17*$U$12+$V$12</f>
+      <c r="Z17" s="73">
+        <f t="shared" si="2"/>
         <v>24.24998171882892</v>
       </c>
-      <c r="AA17" s="1">
-        <f>G17*$U$13+$V$13</f>
+      <c r="AA17" s="73">
+        <f t="shared" si="3"/>
         <v>1.8054143161388794</v>
       </c>
-      <c r="AC17" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD17" s="73">
+        <f t="shared" si="4"/>
         <v>28.224379860627174</v>
       </c>
-      <c r="AD17" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE17" s="73">
+        <f>ABS($C17-Y17)</f>
         <v>31.012033875794216</v>
       </c>
-      <c r="AE17" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF17" s="73">
+        <f>ABS($C17-Z17)</f>
         <v>3.7475914749264803</v>
       </c>
-      <c r="AF17" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG17" s="73">
+        <f>ABS($C17-AA17)</f>
         <v>18.69697592776356</v>
       </c>
     </row>
-    <row r="18" spans="2:32">
+    <row r="18" spans="2:33">
       <c r="B18" s="103">
         <v>17</v>
       </c>
@@ -36719,40 +36782,40 @@
         <v>7.1000000000000005</v>
       </c>
       <c r="H18" s="99"/>
-      <c r="X18" s="1">
-        <f>$D18*$U$10+$V$10</f>
+      <c r="X18" s="73">
+        <f t="shared" si="0"/>
         <v>99.48736501742161</v>
       </c>
-      <c r="Y18" s="1">
-        <f>E18*$U$11+$V$11</f>
+      <c r="Y18" s="73">
+        <f t="shared" si="1"/>
         <v>110.59042467380016</v>
       </c>
-      <c r="Z18" s="1">
-        <f>F18*$U$12+$V$12</f>
+      <c r="Z18" s="73">
+        <f t="shared" si="2"/>
         <v>65.299256866793669</v>
       </c>
-      <c r="AA18" s="1">
-        <f>G18*$U$13+$V$13</f>
+      <c r="AA18" s="73">
+        <f t="shared" si="3"/>
         <v>101.21346397103139</v>
       </c>
-      <c r="AC18" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD18" s="73">
+        <f t="shared" si="4"/>
         <v>0.50104961672474246</v>
       </c>
-      <c r="AD18" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE18" s="73">
+        <f>ABS($C18-Y18)</f>
         <v>10.602010039653806</v>
       </c>
-      <c r="AE18" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF18" s="73">
+        <f>ABS($C18-Z18)</f>
         <v>34.689157767352683</v>
       </c>
-      <c r="AF18" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG18" s="73">
+        <f>ABS($C18-AA18)</f>
         <v>1.2250493368850357</v>
       </c>
     </row>
-    <row r="19" spans="2:32">
+    <row r="19" spans="2:33">
       <c r="B19" s="103">
         <v>19</v>
       </c>
@@ -36774,40 +36837,40 @@
         <v>8.6915907722453642</v>
       </c>
       <c r="H19" s="99"/>
-      <c r="X19" s="1">
-        <f>$D19*$U$10+$V$10</f>
+      <c r="X19" s="73">
+        <f t="shared" si="0"/>
         <v>86.797216289198616</v>
       </c>
-      <c r="Y19" s="1">
-        <f>E19*$U$11+$V$11</f>
+      <c r="Y19" s="73">
+        <f t="shared" si="1"/>
         <v>139.0137834309632</v>
       </c>
-      <c r="Z19" s="1">
-        <f>F19*$U$12+$V$12</f>
+      <c r="Z19" s="73">
+        <f t="shared" si="2"/>
         <v>116.08542007985569</v>
       </c>
-      <c r="AA19" s="1">
-        <f>G19*$U$13+$V$13</f>
+      <c r="AA19" s="73">
+        <f t="shared" si="3"/>
         <v>132.23639230782274</v>
       </c>
-      <c r="AC19" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD19" s="73">
+        <f t="shared" si="4"/>
         <v>58.442612979094093</v>
       </c>
-      <c r="AD19" s="1">
-        <f t="shared" si="0"/>
+      <c r="AE19" s="73">
+        <f>ABS($C19-Y19)</f>
         <v>6.226045837329508</v>
       </c>
-      <c r="AE19" s="1">
-        <f t="shared" si="0"/>
+      <c r="AF19" s="73">
+        <f>ABS($C19-Z19)</f>
         <v>29.154409188437015</v>
       </c>
-      <c r="AF19" s="1">
-        <f t="shared" si="0"/>
+      <c r="AG19" s="73">
+        <f>ABS($C19-AA19)</f>
         <v>13.003436960469969</v>
       </c>
     </row>
-    <row r="20" spans="2:32">
+    <row r="20" spans="2:33">
       <c r="B20" s="103">
         <v>20</v>
       </c>
@@ -36829,40 +36892,40 @@
         <v>6.4580000000000011</v>
       </c>
       <c r="H20" s="99"/>
-      <c r="X20" s="1">
-        <f>$D20*$U$10+$V$10</f>
+      <c r="X20" s="73">
+        <f t="shared" si="0"/>
         <v>99.48736501742161</v>
       </c>
-      <c r="Y20" s="1">
-        <f>E20*$U$11+$V$11</f>
+      <c r="Y20" s="73">
+        <f t="shared" si="1"/>
         <v>74.921896037360312</v>
       </c>
-      <c r="Z20" s="1">
-        <f>F20*$U$12+$V$12</f>
+      <c r="Z20" s="73">
+        <f t="shared" si="2"/>
         <v>81.144277073908071</v>
       </c>
-      <c r="AA20" s="1">
-        <f>G20*$U$13+$V$13</f>
+      <c r="AA20" s="73">
+        <f t="shared" si="3"/>
         <v>88.699744779180236</v>
       </c>
-      <c r="AC20" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD20" s="73">
+        <f t="shared" si="4"/>
         <v>18.865535749128924</v>
       </c>
-      <c r="AD20" s="1">
-        <f t="shared" ref="AD20:AD22" si="3">ABS($C20-Y20)</f>
+      <c r="AE20" s="73">
+        <f t="shared" ref="AE20:AE22" si="6">ABS($C20-Y20)</f>
         <v>5.6999332309323734</v>
       </c>
-      <c r="AE20" s="1">
-        <f t="shared" ref="AE20:AE22" si="4">ABS($C20-Z20)</f>
+      <c r="AF20" s="73">
+        <f t="shared" ref="AF20:AF22" si="7">ABS($C20-Z20)</f>
         <v>0.52244780561538562</v>
       </c>
-      <c r="AF20" s="1">
-        <f t="shared" ref="AF20:AF22" si="5">ABS($C20-AA20)</f>
+      <c r="AG20" s="73">
+        <f t="shared" ref="AG20:AG22" si="8">ABS($C20-AA20)</f>
         <v>8.07791551088755</v>
       </c>
     </row>
-    <row r="21" spans="2:32">
+    <row r="21" spans="2:33">
       <c r="B21" s="103">
         <v>21</v>
       </c>
@@ -36884,40 +36947,40 @@
         <v>6.1128912</v>
       </c>
       <c r="H21" s="102"/>
-      <c r="X21" s="1">
-        <f>$D21*$U$10+$V$10</f>
+      <c r="X21" s="73">
+        <f t="shared" si="0"/>
         <v>74.107067560975608</v>
       </c>
-      <c r="Y21" s="1">
-        <f>E21*$U$11+$V$11</f>
+      <c r="Y21" s="73">
+        <f t="shared" si="1"/>
         <v>85.510990476303391</v>
       </c>
-      <c r="Z21" s="1">
-        <f>F21*$U$12+$V$12</f>
+      <c r="Z21" s="73">
+        <f t="shared" si="2"/>
         <v>71.702943789876173</v>
       </c>
-      <c r="AA21" s="1">
-        <f>G21*$U$13+$V$13</f>
+      <c r="AA21" s="73">
+        <f t="shared" si="3"/>
         <v>81.972961891584063</v>
       </c>
-      <c r="AC21" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD21" s="73">
+        <f t="shared" si="4"/>
         <v>15.832151951219515</v>
       </c>
-      <c r="AD21" s="1">
-        <f t="shared" si="3"/>
+      <c r="AE21" s="73">
+        <f t="shared" si="6"/>
         <v>4.4282290358917322</v>
       </c>
-      <c r="AE21" s="1">
-        <f t="shared" si="4"/>
+      <c r="AF21" s="73">
+        <f t="shared" si="7"/>
         <v>18.23627572231895</v>
       </c>
-      <c r="AF21" s="1">
-        <f t="shared" si="5"/>
+      <c r="AG21" s="73">
+        <f t="shared" si="8"/>
         <v>7.96625762061106</v>
       </c>
     </row>
-    <row r="22" spans="2:32">
+    <row r="22" spans="2:33">
       <c r="B22" s="37">
         <v>23</v>
       </c>
@@ -36939,40 +37002,40 @@
         <v>5.7813413250560011</v>
       </c>
       <c r="H22" s="102"/>
-      <c r="X22" s="1">
-        <f>$D22*$U$10+$V$10</f>
+      <c r="X22" s="73">
+        <f t="shared" si="0"/>
         <v>74.107067560975608</v>
       </c>
-      <c r="Y22" s="1">
-        <f>E22*$U$11+$V$11</f>
+      <c r="Y22" s="73">
+        <f t="shared" si="1"/>
         <v>73.807254517471563</v>
       </c>
-      <c r="Z22" s="1">
-        <f>F22*$U$12+$V$12</f>
+      <c r="Z22" s="73">
+        <f t="shared" si="2"/>
         <v>71.440228428929203</v>
       </c>
-      <c r="AA22" s="1">
-        <f>G22*$U$13+$V$13</f>
+      <c r="AA22" s="73">
+        <f t="shared" si="3"/>
         <v>75.510466512857306</v>
       </c>
-      <c r="AC22" s="1">
-        <f t="shared" si="1"/>
+      <c r="AD22" s="73">
+        <f t="shared" si="4"/>
         <v>19.606360243902451</v>
       </c>
-      <c r="AD22" s="1">
-        <f t="shared" si="3"/>
+      <c r="AE22" s="73">
+        <f t="shared" si="6"/>
         <v>19.306547200398406</v>
       </c>
-      <c r="AE22" s="1">
-        <f t="shared" si="4"/>
+      <c r="AF22" s="73">
+        <f t="shared" si="7"/>
         <v>16.939521111856045</v>
       </c>
-      <c r="AF22" s="1">
-        <f t="shared" si="5"/>
+      <c r="AG22" s="73">
+        <f t="shared" si="8"/>
         <v>21.009759195784149</v>
       </c>
     </row>
-    <row r="23" spans="2:32">
+    <row r="23" spans="2:33">
       <c r="C23" s="74" t="s">
         <v>326</v>
       </c>
@@ -36993,24 +37056,27 @@
         <v>0.93180506545250352</v>
       </c>
       <c r="H23" s="99"/>
-      <c r="AC23" s="122">
-        <f>AVERAGE(AC4:AC22)</f>
+      <c r="AC23" s="127" t="s">
+        <v>483</v>
+      </c>
+      <c r="AD23" s="127">
+        <f>AVERAGE(AD4:AD22)</f>
         <v>26.770956059050064</v>
       </c>
-      <c r="AD23" s="122">
-        <f>AVERAGE(AD4:AD22)</f>
+      <c r="AE23" s="127">
+        <f>AVERAGE(AE4:AE22)</f>
         <v>25.68456665394233</v>
       </c>
-      <c r="AE23" s="122">
-        <f t="shared" ref="AE23:AF23" si="6">AVERAGE(AE4:AE22)</f>
+      <c r="AF23" s="127">
+        <f t="shared" ref="AF23:AG23" si="9">AVERAGE(AF4:AF22)</f>
         <v>16.263023807354067</v>
       </c>
-      <c r="AF23" s="122">
-        <f t="shared" si="6"/>
+      <c r="AG23" s="127">
+        <f t="shared" si="9"/>
         <v>13.532561849160183</v>
       </c>
     </row>
-    <row r="24" spans="2:32" hidden="1">
+    <row r="24" spans="2:33" hidden="1">
       <c r="C24" s="74" t="s">
         <v>327</v>
       </c>
@@ -37021,382 +37087,416 @@
       </c>
       <c r="G24" s="74"/>
       <c r="H24" s="99"/>
-    </row>
-    <row r="25" spans="2:32" ht="350" customHeight="1"/>
-    <row r="26" spans="2:32">
-      <c r="B26" s="107" t="s">
+      <c r="AC24" s="73"/>
+      <c r="AD24" s="73"/>
+      <c r="AE24" s="73"/>
+      <c r="AF24" s="73"/>
+      <c r="AG24" s="73"/>
+    </row>
+    <row r="25" spans="2:33">
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
+      <c r="E25" s="123"/>
+      <c r="F25" s="123"/>
+      <c r="G25" s="123"/>
+      <c r="H25" s="99"/>
+      <c r="AC25" s="128" t="s">
+        <v>508</v>
+      </c>
+      <c r="AD25" s="128">
+        <f>STDEV(AD4:AD22)</f>
+        <v>26.449508599507176</v>
+      </c>
+      <c r="AE25" s="128">
+        <f t="shared" ref="AE25:AG25" si="10">STDEV(AE4:AE22)</f>
+        <v>27.660337593421776</v>
+      </c>
+      <c r="AF25" s="128">
+        <f t="shared" si="10"/>
+        <v>13.547304105814254</v>
+      </c>
+      <c r="AG25" s="128">
+        <f t="shared" si="10"/>
+        <v>9.2392948821241667</v>
+      </c>
+    </row>
+    <row r="26" spans="2:33" ht="350" customHeight="1"/>
+    <row r="27" spans="2:33">
+      <c r="B27" s="109" t="s">
         <v>505</v>
       </c>
-      <c r="C26" s="107"/>
-      <c r="D26" s="107"/>
-      <c r="E26" s="107"/>
-    </row>
-    <row r="28" spans="2:32">
-      <c r="B28" s="72" t="s">
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+    </row>
+    <row r="29" spans="2:33">
+      <c r="B29" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="72" t="s">
+      <c r="C29" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="72" t="s">
+      <c r="D29" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="72" t="s">
+      <c r="E29" s="72" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:32">
-      <c r="B29" s="73">
+    <row r="30" spans="2:33">
+      <c r="B30" s="73">
         <v>1</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C30" s="36">
         <v>68.014414634146334</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D30" s="37">
         <v>1</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E30" s="37">
         <v>6.8</v>
       </c>
     </row>
-    <row r="30" spans="2:32">
-      <c r="B30" s="73">
+    <row r="31" spans="2:33">
+      <c r="B31" s="73">
         <v>2</v>
       </c>
-      <c r="C30" s="36">
+      <c r="C31" s="36">
         <v>100.26741463414632</v>
-      </c>
-      <c r="D30" s="37">
-        <v>5</v>
-      </c>
-      <c r="E30" s="37">
-        <v>18.100000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="2:32">
-      <c r="B31" s="73">
-        <v>3</v>
-      </c>
-      <c r="C31" s="36">
-        <v>132.46873170731703</v>
       </c>
       <c r="D31" s="37">
         <v>5</v>
       </c>
       <c r="E31" s="37">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="2:33">
+      <c r="B32" s="73">
+        <v>3</v>
+      </c>
+      <c r="C32" s="36">
+        <v>132.46873170731703</v>
+      </c>
+      <c r="D32" s="37">
+        <v>5</v>
+      </c>
+      <c r="E32" s="37">
         <v>12.8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:32">
-      <c r="B32" s="73">
-        <v>4</v>
-      </c>
-      <c r="C32" s="36">
-        <v>154.64156097560979</v>
-      </c>
-      <c r="D32" s="37">
-        <v>7</v>
-      </c>
-      <c r="E32" s="37">
-        <v>15.4</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="73">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" s="36">
-        <v>211.48453658536584</v>
+        <v>154.64156097560979</v>
       </c>
       <c r="D33" s="37">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E33" s="37">
-        <v>14.3</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="73">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" s="36">
-        <v>70.510951219512179</v>
+        <v>211.48453658536584</v>
       </c>
       <c r="D34" s="37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E34" s="37">
-        <v>7.1</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="73">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="36">
-        <v>66.048609756097534</v>
+        <v>70.510951219512179</v>
       </c>
       <c r="D35" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E35" s="37">
-        <v>9.5</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="73">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" s="36">
-        <v>104.82602439024393</v>
+        <v>66.048609756097534</v>
       </c>
       <c r="D36" s="37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E36" s="37">
-        <v>7.4</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="73">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="36">
-        <v>65.420853658536572</v>
+        <v>104.82602439024393</v>
       </c>
       <c r="D37" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" s="37">
-        <v>8.9</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="73">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" s="36">
-        <v>42.585804878048783</v>
+        <v>65.420853658536572</v>
       </c>
       <c r="D38" s="37">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E38" s="37">
-        <v>16.7</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="73">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C39" s="36">
-        <v>65.473780487804873</v>
+        <v>42.585804878048783</v>
       </c>
       <c r="D39" s="37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E39" s="37">
-        <v>7.4</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="73">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40" s="36">
-        <v>59.81002439024391</v>
+        <v>65.473780487804873</v>
       </c>
       <c r="D40" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40" s="37">
-        <v>14</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="B41" s="73">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" s="36">
-        <v>37.425292682926823</v>
+        <v>59.81002439024391</v>
       </c>
       <c r="D41" s="37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E41" s="37">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="B42" s="73">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42" s="36">
-        <v>48.394707317073163</v>
+        <v>37.425292682926823</v>
       </c>
       <c r="D42" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="37">
-        <v>9.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="B43" s="73">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43" s="36">
-        <v>355.30917073170724</v>
+        <v>48.394707317073163</v>
       </c>
       <c r="D43" s="37">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E43" s="37">
-        <v>29.7</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="73">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C44" s="36">
-        <v>20.50239024390244</v>
+        <v>355.30917073170724</v>
       </c>
       <c r="D44" s="37">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E44" s="37">
-        <v>5.6</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="73">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C45" s="36">
-        <v>99.988414634146352</v>
+        <v>20.50239024390244</v>
       </c>
       <c r="D45" s="37">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E45" s="37">
-        <v>16.2</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="73">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="36">
-        <v>132.07892682926831</v>
+        <v>99.988414634146352</v>
       </c>
       <c r="D46" s="37">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E46" s="37">
-        <v>16.7</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="B47" s="73">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C47" s="36">
-        <v>145.23982926829271</v>
+        <v>132.07892682926831</v>
       </c>
       <c r="D47" s="37">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E47" s="37">
-        <v>21.3</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="B48" s="73">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48" s="36">
-        <v>80.621829268292686</v>
+        <v>145.23982926829271</v>
       </c>
       <c r="D48" s="37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" s="37">
-        <v>9.8000000000000007</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="49" spans="2:5">
       <c r="B49" s="73">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C49" s="36">
-        <v>89.939219512195123</v>
+        <v>80.621829268292686</v>
       </c>
       <c r="D49" s="37">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E49" s="37">
-        <v>11.7</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="73">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C50" s="36">
-        <v>86.29456097560977</v>
+        <v>89.939219512195123</v>
       </c>
       <c r="D50" s="37">
         <v>2</v>
       </c>
       <c r="E50" s="37">
-        <v>10.6</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="73">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="36">
-        <v>54.500707317073157</v>
+        <v>86.29456097560977</v>
       </c>
       <c r="D51" s="37">
         <v>2</v>
       </c>
       <c r="E51" s="37">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" s="73">
+        <v>23</v>
+      </c>
+      <c r="C52" s="36">
+        <v>54.500707317073157</v>
+      </c>
+      <c r="D52" s="37">
+        <v>2</v>
+      </c>
+      <c r="E52" s="37">
         <v>9.6</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
-      <c r="C52" s="74" t="s">
-        <v>326</v>
-      </c>
-      <c r="D52" s="74">
-        <f>PEARSON($C29:$C51,D29:D51)</f>
-        <v>0.72591509307923441</v>
-      </c>
-      <c r="E52" s="74">
-        <f>PEARSON($C29:$C51,E29:E51)</f>
-        <v>0.78748899109661075</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="C53" s="74" t="s">
+        <v>326</v>
+      </c>
+      <c r="D53" s="74">
+        <f>PEARSON($C30:$C52,D30:D52)</f>
+        <v>0.72591509307923441</v>
+      </c>
+      <c r="E53" s="74">
+        <f>PEARSON($C30:$C52,E30:E52)</f>
+        <v>0.78748899109661075</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="C54" s="74" t="s">
         <v>327</v>
       </c>
-      <c r="D53" s="38">
+      <c r="D54" s="38">
         <v>0.50800000000000001</v>
       </c>
-      <c r="E53" s="38">
+      <c r="E54" s="38">
         <v>0.48499999999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B26:E26"/>
+  <mergeCells count="6">
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="B27:E27"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="T9:V9"/>
+    <mergeCell ref="X2:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -37419,26 +37519,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="121" t="s">
         <v>240</v>
       </c>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="15"/>
@@ -37741,14 +37841,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="120"/>
     </row>
     <row r="3" spans="1:8">
       <c r="F3" s="42">
@@ -38389,13 +38489,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="18"/>
@@ -38715,13 +38815,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
     </row>
     <row r="3" spans="1:7">
       <c r="E3" s="42">
@@ -39037,12 +39137,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
     </row>
     <row r="2" spans="1:6" s="10" customFormat="1"/>
     <row r="3" spans="1:6" s="10" customFormat="1">
@@ -39508,7 +39608,7 @@
   <sheetPr codeName="Feuil64"/>
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4:G19"/>
     </sheetView>
   </sheetViews>
@@ -39523,13 +39623,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="19">
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="108" t="s">
         <v>475</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="72" t="s">
@@ -39971,36 +40071,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="19">
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="108" t="s">
         <v>501</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+      <c r="G1" s="108"/>
+      <c r="H1" s="108"/>
     </row>
     <row r="3" spans="2:8">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="110" t="s">
         <v>471</v>
       </c>
-      <c r="C3" s="109"/>
-      <c r="E3" s="112" t="s">
+      <c r="C3" s="111"/>
+      <c r="E3" s="114" t="s">
         <v>480</v>
       </c>
       <c r="F3" s="72" t="s">
         <v>500</v>
       </c>
-      <c r="G3" s="114" t="s">
+      <c r="G3" s="116" t="s">
         <v>326</v>
       </c>
-      <c r="H3" s="114"/>
+      <c r="H3" s="116"/>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="110"/>
-      <c r="C4" s="111"/>
-      <c r="E4" s="113"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="113"/>
+      <c r="E4" s="115"/>
       <c r="F4" s="72"/>
       <c r="G4" s="72" t="s">
         <v>503</v>
@@ -40109,14 +40209,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
     </row>
     <row r="3" spans="1:11">
       <c r="B3" s="78"/>
@@ -40559,16 +40659,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="3" spans="1:9">
       <c r="G3" s="29">
@@ -41652,16 +41752,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="22"/>

</xml_diff>